<commit_message>
descriptive statistics q 2:4
</commit_message>
<xml_diff>
--- a/03-descriptive statistics/descriptive-statistics.xlsx
+++ b/03-descriptive statistics/descriptive-statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\statistics-4-data-science-business-analysis\03-descriptive statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5F02A0-9A4F-4A7B-A13F-FBE34179D6FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209F1F7F-AD3A-4BF9-8BF4-439DB2FEBA3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="365RE" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,15 @@
     <sheet name="Tasks 6,7" sheetId="10" r:id="rId5"/>
     <sheet name="Tasks 8,9" sheetId="5" r:id="rId6"/>
     <sheet name="Task 10" sheetId="6" r:id="rId7"/>
+    <sheet name="histo test" sheetId="11" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'365RE'!$A$5:$AM$926</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'365RE'!$I$6:$I$272</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'365RE'!$I$6:$I$272</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'365RE'!$I$6:$I$272</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'365RE'!$I$6:$I$272</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Tasks 2,3,4'!$B$20:$B$24</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -38,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2513" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2517" uniqueCount="561">
   <si>
     <t>Office</t>
   </si>
@@ -1852,6 +1858,12 @@
   </si>
   <si>
     <t>Quantitative --&gt; Interval</t>
+  </si>
+  <si>
+    <t>min price</t>
+  </si>
+  <si>
+    <t>max price</t>
   </si>
 </sst>
 </file>
@@ -2017,7 +2029,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2138,9 +2150,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2154,6 +2163,13 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2191,6 +2207,1335 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{9288D21D-CE68-4982-82F4-112E2943E5E7}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r">
+              <cx:binSize val="100000"/>
+            </cx:binning>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.3</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{F4295C6A-6146-4B60-878F-20B1AFFC0F52}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r">
+              <cx:binCount val="267"/>
+            </cx:binning>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>115047</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>105709</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>314699</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>105709</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{818B1D04-7094-4786-3622-2B81BCD6FD7D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9306672" y="1372534"/>
+              <a:ext cx="4924052" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Chart 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BEBC6A8-E376-34F2-B528-AC9F70EB6DA8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3590925" y="1262062"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2493,8 +3838,8 @@
   <dimension ref="A1:AA920"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <pane ySplit="5" topLeftCell="A247" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6:I272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2547,35 +3892,35 @@
       <c r="W3" s="14"/>
     </row>
     <row r="4" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="51" t="s">
         <v>528</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="L4" s="46" t="s">
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="L4" s="51" t="s">
         <v>529</v>
       </c>
-      <c r="M4" s="46"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="46"/>
-      <c r="S4" s="46"/>
-      <c r="T4" s="46"/>
-      <c r="U4" s="46"/>
-      <c r="V4" s="46"/>
-      <c r="W4" s="46"/>
-      <c r="X4" s="46"/>
-      <c r="Y4" s="46"/>
-      <c r="Z4" s="46"/>
-      <c r="AA4" s="46"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="51"/>
+      <c r="S4" s="51"/>
+      <c r="T4" s="51"/>
+      <c r="U4" s="51"/>
+      <c r="V4" s="51"/>
+      <c r="W4" s="51"/>
+      <c r="X4" s="51"/>
+      <c r="Y4" s="51"/>
+      <c r="Z4" s="51"/>
+      <c r="AA4" s="51"/>
     </row>
     <row r="5" spans="2:27" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="35" t="s">
@@ -21273,8 +22618,13 @@
       <c r="E274" s="4"/>
       <c r="F274" s="1"/>
       <c r="G274" s="1"/>
-      <c r="H274" s="2"/>
-      <c r="I274" s="2"/>
+      <c r="H274" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="I274" s="2">
+        <f>MIN($I$6:$I$272)</f>
+        <v>117564.0716</v>
+      </c>
       <c r="J274" s="2"/>
       <c r="K274" s="2"/>
       <c r="L274" s="8"/>
@@ -21302,8 +22652,13 @@
       <c r="E275" s="4"/>
       <c r="F275" s="1"/>
       <c r="G275" s="1"/>
-      <c r="H275" s="2"/>
-      <c r="I275" s="37"/>
+      <c r="H275" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="I275" s="37">
+        <f>MAX($I$6:$I$272)</f>
+        <v>538271.73560000001</v>
+      </c>
       <c r="J275" s="2"/>
       <c r="K275" s="2"/>
       <c r="L275" s="8"/>
@@ -40071,7 +41426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A7C1412-EA0B-443B-AF04-4E1F30BE9CF6}">
   <dimension ref="B1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -40106,43 +41461,43 @@
     </row>
     <row r="6" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B6" s="26"/>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="46" t="s">
         <v>552</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="47" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="48" t="s">
         <v>551</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="50" t="s">
         <v>554</v>
       </c>
-      <c r="D7" s="51" t="s">
+      <c r="D7" s="50" t="s">
         <v>555</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="50" t="s">
         <v>556</v>
       </c>
-      <c r="D8" s="51" t="s">
+      <c r="D8" s="50" t="s">
         <v>555</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="50" t="s">
         <v>557</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="50" t="s">
         <v>558</v>
       </c>
     </row>
@@ -40160,16 +41515,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988EDBF6-8135-42D7-A181-4E7F0B86819A}">
-  <dimension ref="B1:D8"/>
+  <dimension ref="B1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2" style="32" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" style="32" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="32" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" style="32" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" style="32" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.85546875" style="32"/>
@@ -40216,12 +41571,52 @@
       <c r="C8" s="28"/>
       <c r="D8" s="27"/>
     </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="C10" s="52">
+        <f>MIN('365RE'!$I$6:$I$272)</f>
+        <v>117564.0716</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="C11" s="52">
+        <f>MAX('365RE'!$I$6:$I$272)</f>
+        <v>538271.73560000001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C16" s="53"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="53"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="53"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="53"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="53"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" s="53"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="53"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="B1:B2" xr:uid="{B1FC3192-AC7F-4321-8673-4F49FE1F8C37}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -41527,4 +42922,16 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA03805-5E70-419D-84D6-7644FB053147}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
descriptive statistics q 5
</commit_message>
<xml_diff>
--- a/03-descriptive statistics/descriptive-statistics.xlsx
+++ b/03-descriptive statistics/descriptive-statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\statistics-4-data-science-business-analysis\03-descriptive statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209F1F7F-AD3A-4BF9-8BF4-439DB2FEBA3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA05C223-F2A0-42FE-ACBA-430EC3BB54A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="365RE" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'365RE'!$A$5:$AM$926</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">'365RE'!$I$6:$I$272</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'365RE'!$I$6:$I$272</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'365RE'!$I$6:$I$272</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'365RE'!$I$6:$I$272</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Tasks 2,3,4'!$B$20:$B$24</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -44,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2517" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2519" uniqueCount="563">
   <si>
     <t>Office</t>
   </si>
@@ -1864,6 +1861,12 @@
   </si>
   <si>
     <t>max price</t>
+  </si>
+  <si>
+    <t>The correlation coefficient</t>
+  </si>
+  <si>
+    <t>The scatter plot and the correlation coefficient show a very strong linear relationship between Price and Area.</t>
   </si>
 </sst>
 </file>
@@ -2029,7 +2032,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2163,13 +2166,14 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2207,6 +2211,2043 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Price &amp; Area Relationship</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'365RE'!$I$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Price</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'365RE'!$H$6:$H$272</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="267"/>
+                <c:pt idx="0">
+                  <c:v>743.0856</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>756.21280000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>587.2808</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1604.7463999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1375.4507999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>675.18999999999994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>670.88599999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>720.81239999999991</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>782.25200000000007</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>794.51840000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1160.3584000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1942.5028</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>794.51840000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1109.2483999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1400.9519999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1479.7152000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>790.53719999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>723.93280000000004</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>781.0684</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1127.7556</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>720.70479999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>649.68880000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1307.4476</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>618.37720000000002</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>625.80160000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1203.2908</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>670.88599999999997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1434.0927999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>781.0684</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1596.3536000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1110.3244</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>781.0684</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>697.89359999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>625.80160000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>957.53239999999994</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>722.96439999999996</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>923.20799999999997</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>670.24040000000002</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>785.48</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>798.28440000000001</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1121.9451999999999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>782.25200000000007</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>923.20799999999997</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1434.0927999999999</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1160.3584000000001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>798.28440000000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>733.18639999999994</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>798.28440000000001</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>733.18639999999994</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>717.04639999999995</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>747.49720000000002</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1121.9451999999999</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1121.9451999999999</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>827.87439999999992</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>747.49720000000002</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1608.8352</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1132.0595999999998</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1383.8436000000002</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>927.83479999999997</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>669.1644</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>928.1576</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>798.49959999999987</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1305.6184000000001</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1121.9451999999999</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>785.48</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>927.08159999999998</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1109.2483999999999</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>649.79639999999995</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>785.48</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1596.3536000000001</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1121.9451999999999</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>743.40840000000003</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>756.21280000000002</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>649.79639999999995</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>785.48</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>785.48</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1283.4528</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1434.0927999999999</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>782.25200000000007</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1288.6176</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>781.0684</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1222.336</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>781.0684</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>743.0856</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>785.48</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1109.2483999999999</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>579.74879999999996</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1128.4012</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>701.65959999999995</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1336.93</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>794.51840000000004</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1171.5488</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>794.51840000000004</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>798.28440000000001</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>798.28440000000001</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>649.79639999999995</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1137.4395999999999</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1604.7463999999998</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>675.18999999999994</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>649.68880000000001</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>785.48</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>781.0684</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>1127.7556</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>794.51840000000004</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>794.51840000000004</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>781.0684</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>720.81239999999991</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>927.83479999999997</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>927.83479999999997</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>785.48</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>618.16200000000003</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1109.2483999999999</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>720.70479999999998</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>720.81239999999991</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>927.08159999999998</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>798.28440000000001</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1057.9232</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>781.0684</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1396.8632</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>794.51840000000004</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>923.20799999999997</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>781.0684</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>782.25200000000007</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>733.18639999999994</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>733.18639999999994</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>794.51840000000004</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>756.21280000000002</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>736.62959999999987</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>785.48</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>781.0684</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>798.28440000000001</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>798.28440000000001</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>827.87439999999992</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>1160.3584000000001</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>827.87439999999992</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>723.8252</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>798.28440000000001</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>1238.5835999999999</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>723.8252</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>977.86879999999996</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>1093.0008</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>927.83479999999997</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>701.65959999999995</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>680.56999999999994</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>723.93280000000004</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>649.79639999999995</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>649.79639999999995</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>785.48</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>785.48</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>1615.2912000000001</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>1132.0595999999998</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>720.38200000000006</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>733.18639999999994</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>782.25200000000007</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>798.28440000000001</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>1057.9232</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>723.8252</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>798.28440000000001</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>794.51840000000004</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>794.51840000000004</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>782.25200000000007</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>785.48</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>923.20799999999997</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>923.20799999999997</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>1434.0927999999999</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>782.25200000000007</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>781.0684</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>618.37720000000002</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>923.20799999999997</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>781.0684</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>781.0684</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>781.0684</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>697.89359999999999</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>670.88599999999997</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>782.25200000000007</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>743.40840000000003</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>923.20799999999997</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>923.20799999999997</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>1769.4819999999997</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>410.70920000000001</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>1200.82</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>800.96</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>827.87439999999992</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>775.6884</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>775.6884</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>1604.7463999999998</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>587.2808</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>756.21280000000002</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>743.0856</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>827.87439999999992</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>1160.3584000000001</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>743.0856</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>1160.3584000000001</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>625.80160000000001</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>756.21280000000002</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>625.80160000000001</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>1238.5835999999999</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>713.71079999999995</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>763.20680000000004</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>798.49959999999987</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>618.37720000000002</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>1479.7152000000001</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>1603.9931999999999</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>1615.2912000000001</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>784.1887999999999</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>720.38200000000006</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>1596.3536000000001</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>1121.9451999999999</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>1596.3536000000001</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>1596.3536000000001</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>1273.8763999999999</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>966.57079999999996</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>1357.1587999999999</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>1343.386</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>758.68760000000009</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>789.24599999999987</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>789.24599999999987</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>733.18639999999994</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>1611.8480000000002</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>789.24599999999987</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>1611.8480000000002</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>789.24599999999987</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>794.51840000000004</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>1611.8480000000002</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>789.24599999999987</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>794.51840000000004</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>1611.8480000000002</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>789.24599999999987</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>794.51840000000004</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>1111.7231999999999</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>785.48</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>1058.2459999999999</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>791.72079999999994</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>1068.5755999999999</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>1325.3091999999999</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>1273.8763999999999</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>798.49959999999987</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>798.49959999999987</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>798.49959999999987</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>1058.2459999999999</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>618.16200000000003</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>1273.8763999999999</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>798.49959999999987</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>798.49959999999987</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>798.49959999999987</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>1058.2459999999999</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>1273.5536</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>798.49959999999987</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>798.49959999999987</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>798.28440000000001</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>1057.9232</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>1273.5536</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>618.16200000000003</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>1273.5536</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>1057.9232</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>1273.5536</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>798.28440000000001</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>1057.9232</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>606.32600000000002</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>1273.5536</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>798.28440000000001</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>598.5788</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>1238.5835999999999</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>794.51840000000004</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>1013.2692</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>1074.7087999999999</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>789.24599999999987</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'365RE'!$I$6:$I$272</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="267"/>
+                <c:pt idx="0">
+                  <c:v>246172.67600000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>246331.90400000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>209280.91039999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>452667.00639999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>467083.31319999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>203491.84999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>212520.826</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>198591.84879999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>265467.68000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>235633.2592</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>317473.86080000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>503790.23080000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>217786.37600000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>460001.25599999994</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>460001.25599999994</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>448134.26880000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>249591.99479999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>196142.19200000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>258572.47760000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>310831.21159999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>207281.5912</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>168834.04240000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>396973.83240000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>188743.1072</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>179674.07519999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>306363.64360000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>200300.63399999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>382041.12799999997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>245572.7936</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>407214.28960000002</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>355073.4032</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>256821.6404</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>226342.80319999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>191389.8688</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>297008.96519999998</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>250773.1452</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>312211.14399999997</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>190119.50400000002</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>225050.52000000002</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>261742.742</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>344530.88879999996</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>215410.27600000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>252185.992</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>480545.80959999998</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>300385.6176</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>240539.34760000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>222138.71599999999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>228410.054</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>197053.51439999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>193660.62079999998</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>237060.1488</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>372001.69679999998</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>290031.25879999995</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>238811.06399999998</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>199054.1992</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>496266.40639999998</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>346906.89319999993</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>376964.61560000002</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>315733.15360000002</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>188273.7304</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>253831.02480000001</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>278575.86879999994</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>402081.79600000003</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>310832.58759999997</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>257183.48</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>326885.33600000001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>344568.74280000001</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>214631.68039999998</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>237207.67999999999</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>464549.19040000002</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>310577.03959999996</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>205098.2108</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>248525.11680000002</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>224463.86599999998</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>220606.28</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>220865</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>338181.18080000003</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>432679.91199999995</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>196220.04800000001</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>323915.8112</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>200719.01519999999</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>380809.52</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>213942.5624</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>207581.42720000001</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>241671.52000000002</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>336695.2524</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>171262.6544</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>299159.1384</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>212265.66799999998</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>388515.14</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>263790.81440000003</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>367976.45760000002</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>243052.59039999999</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>269075.30160000001</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>223577.32</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>198075.992</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>354553.23239999998</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>456919.45599999995</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>233142.8</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>225401.6152</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>195153.16</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>206631.81</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>358525.59239999996</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>223917.33600000001</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>201518.89440000002</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>269278.57199999999</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>204808.16039999996</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>306878.45759999997</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>275394.24839999998</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>192092.24</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>165430.28200000001</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>310223.29079999996</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>231552.32559999998</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>215774.28439999997</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>289727.99040000001</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>195874.94399999999</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>357538.19519999996</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>239248.7512</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>382277.14880000002</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>248422.66399999999</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>242740.65599999999</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>253025.77720000001</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>234172.38800000004</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>200678.75119999997</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>226578.51199999999</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>200148.89440000002</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>218585.92480000001</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>198841.69519999996</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>252927.84</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>225290.22039999999</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>234750.58600000001</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>287466.41159999999</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>229464.71119999999</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>377313.5552</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>276759.18</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>219373.4056</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>230216.21919999999</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>410932.67319999996</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>214341.3364</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>248274.31359999999</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>390494.27120000002</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>293876.27480000001</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>204286.66679999998</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>230154.52999999997</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>228170.02560000002</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>205085.40479999999</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>177555.06399999998</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>217748.48000000001</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>247739.44</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>484458.03040000005</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>356506.36999999994</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>197869.36400000003</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>236608.95279999997</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>208930.81200000001</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>263123.42080000002</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>286433.57279999997</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>229581.7836</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>252053.0264</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>244820.66720000003</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>241620.48320000002</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>235762.34000000003</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>236639.56</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>294807.64799999999</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>293828.68799999997</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>412856.56159999996</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>224076.83600000001</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>258015.61439999999</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>153466.71240000002</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>261871.696</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>210038.6992</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>210824.0576</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>249075.6568</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>219865.76079999999</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>204292.49399999998</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>261579.89200000002</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>222867.42080000002</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>291494.36</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>296483.14399999997</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>532877.38399999996</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>117564.0716</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>317196.39999999997</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>264142.16000000003</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>222947.20879999999</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>250312.5344</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>246050.40400000001</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>529317.28319999995</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>169158.29440000001</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>206958.712</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>206445.42319999999</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>239341.58079999997</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>398903.42240000004</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>210745.16639999999</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>331154.87840000005</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>204434.6784</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>189194.30720000001</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>204027.0912</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>400865.91599999997</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>217787.71039999998</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>219630.90120000002</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>244624.87199999997</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>163162.8792</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>401302.81920000003</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>538271.73560000001</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>461464.99200000003</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>275812.49280000001</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>216552.71200000003</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>495570.44480000006</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>388656.80639999994</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>495024.09120000002</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>526947.16320000007</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>427236.09959999996</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>327044.36839999998</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>385447.68719999999</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>401894.81799999997</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>264275.78240000003</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>231348.92799999996</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>264238.94999999995</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>217357.63279999999</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>482404.31200000003</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>228937.89599999995</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>498994.03200000006</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>256376.27599999995</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>255243.10879999999</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>506786.66400000005</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>233172.48999999996</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>233834.00480000002</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>523373.44800000009</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>228872.91199999995</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>208655.6704</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>322952.55839999998</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>216826</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>298730.40399999998</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>230495.00639999998</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>346048.04079999996</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>377043.5956</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>413761.70639999997</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>212644.39479999998</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>250415.38199999995</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>219252.89199999996</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>264011.69799999997</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>211406.86800000002</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>396330.29079999996</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>227072.87839999996</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>276323.86559999996</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>230943.37959999996</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>315382.11</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>372016.56160000002</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>237680.87519999995</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>234032.88399999996</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>273165.57680000004</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>271227.49439999997</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>349865.22239999997</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>199730.734</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>338482.45439999999</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>351304.57759999996</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>338472.13279999996</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>212916.35680000001</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>308660.80319999997</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>147343.69400000002</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>448574.6704</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>255337.89800000002</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>175773.58559999999</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>322610.73919999995</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>279191.25599999999</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>287996.52960000001</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>365868.77759999997</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>199216.40399999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-76AD-428D-9373-B8F2606EA105}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="513175336"/>
+        <c:axId val="513185504"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="513175336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="300"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Area</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="513185504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="513185504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="100000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Price</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="513175336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2250,7 +4291,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2322,6 +4363,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3377,6 +5458,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3533,6 +6130,47 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>6</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>559921</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCC88996-3B0C-1D02-2F61-62F73B25D03B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3839,7 +6477,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A247" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6:I272"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5:I272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3892,35 +6530,35 @@
       <c r="W3" s="14"/>
     </row>
     <row r="4" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="53" t="s">
         <v>528</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="L4" s="51" t="s">
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="L4" s="53" t="s">
         <v>529</v>
       </c>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="51"/>
-      <c r="S4" s="51"/>
-      <c r="T4" s="51"/>
-      <c r="U4" s="51"/>
-      <c r="V4" s="51"/>
-      <c r="W4" s="51"/>
-      <c r="X4" s="51"/>
-      <c r="Y4" s="51"/>
-      <c r="Z4" s="51"/>
-      <c r="AA4" s="51"/>
+      <c r="M4" s="53"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="53"/>
+      <c r="P4" s="53"/>
+      <c r="Q4" s="53"/>
+      <c r="R4" s="53"/>
+      <c r="S4" s="53"/>
+      <c r="T4" s="53"/>
+      <c r="U4" s="53"/>
+      <c r="V4" s="53"/>
+      <c r="W4" s="53"/>
+      <c r="X4" s="53"/>
+      <c r="Y4" s="53"/>
+      <c r="Z4" s="53"/>
+      <c r="AA4" s="53"/>
     </row>
     <row r="5" spans="2:27" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="35" t="s">
@@ -41517,7 +44155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988EDBF6-8135-42D7-A181-4E7F0B86819A}">
   <dimension ref="B1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -41575,7 +44213,7 @@
       <c r="B10" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="C10" s="52">
+      <c r="C10" s="51">
         <f>MIN('365RE'!$I$6:$I$272)</f>
         <v>117564.0716</v>
       </c>
@@ -41584,31 +44222,31 @@
       <c r="B11" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="C11" s="52">
+      <c r="C11" s="51">
         <f>MAX('365RE'!$I$6:$I$272)</f>
         <v>538271.73560000001</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C16" s="53"/>
+      <c r="C16" s="52"/>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="53"/>
+      <c r="B20" s="52"/>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" s="53"/>
+      <c r="B21" s="52"/>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="53"/>
+      <c r="B22" s="52"/>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" s="53"/>
+      <c r="B23" s="52"/>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" s="53"/>
+      <c r="B24" s="52"/>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B25" s="53"/>
+      <c r="B25" s="52"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -41622,10 +44260,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC30D9D-B362-4C01-82F7-1CA90CE5A76C}">
-  <dimension ref="B1:D5"/>
+  <dimension ref="B1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -41657,12 +44295,33 @@
       <c r="C5" s="39"/>
       <c r="D5" s="39"/>
     </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="32" t="s">
+        <v>561</v>
+      </c>
+      <c r="D8" s="32">
+        <f>CORREL('365RE'!H6:H272,'365RE'!I6:I272)</f>
+        <v>0.95108737743161964</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D11" s="54"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D12" s="54"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B31" s="32" t="s">
+        <v>562</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="B1:B2" xr:uid="{28797BD3-DDBC-4B39-8885-EAD538643DE2}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
descriptive statistics q 8-9
</commit_message>
<xml_diff>
--- a/03-descriptive statistics/descriptive-statistics.xlsx
+++ b/03-descriptive statistics/descriptive-statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\statistics-4-data-science-business-analysis\03-descriptive statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF09E87-5779-4D8E-BE70-3A22CF42ACC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728C0DC7-63B6-462A-86BB-38C46B74AA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="365RE" sheetId="1" r:id="rId1"/>
@@ -26,21 +26,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'365RE'!$A$5:$AM$926</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">'365RE'!$I$6:$I$272</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'365RE'!$I$6:$I$272</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Tasks 6,7'!$C$8:$C$15</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'Tasks 6,7'!$D$7</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'Tasks 6,7'!$D$8:$D$15</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">'Tasks 6,7'!$B$8:$B$15</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Tasks 6,7'!$C$7</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Tasks 6,7'!$C$8:$C$15</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Tasks 6,7'!$D$7</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Tasks 6,7'!$D$8:$D$15</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Tasks 6,7'!$E$8:$E$15</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Tasks 6,7'!$B$8:$B$15</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Tasks 6,7'!$C$7</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Tasks 6,7'!$C$8:$C$15</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Tasks 6,7'!$D$8:$D$15</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Tasks 6,7'!$E$8:$E$15</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId9"/>
+    <pivotCache cacheId="3" r:id="rId9"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -55,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2560" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2567" uniqueCount="587">
   <si>
     <t>Office</t>
   </si>
@@ -1932,6 +1925,27 @@
   </si>
   <si>
     <t>Cumulative frequency</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>skewness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variance </t>
+  </si>
+  <si>
+    <t>standard deviation</t>
+  </si>
+  <si>
+    <t>We will only comment on the skew, as it is a bit tougher. The skew is right (positive). This means that most properties are relatively cheap with a tiny portion that is more expensive.</t>
   </si>
 </sst>
 </file>
@@ -2242,9 +2256,6 @@
     </xf>
     <xf numFmtId="44" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2274,6 +2285,9 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -4356,7 +4370,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4392,7 +4406,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4431,7 +4445,7 @@
         <cx:f>_xlchart.v1.2</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
@@ -4439,7 +4453,7 @@
         <cx:f>_xlchart.v1.2</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
@@ -4447,7 +4461,7 @@
         <cx:f>_xlchart.v1.2</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -10623,7 +10637,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DF112065-EABF-45BF-A1FE-F19B866AD767}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DF112065-EABF-45BF-A1FE-F19B866AD767}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField dataField="1" showAll="0"/>
@@ -11008,9 +11022,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA920"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
+    <sheetView showGridLines="0" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A247" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11064,35 +11078,35 @@
       <c r="W3" s="14"/>
     </row>
     <row r="4" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="67" t="s">
         <v>528</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="L4" s="54" t="s">
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="L4" s="67" t="s">
         <v>529</v>
       </c>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54"/>
-      <c r="O4" s="54"/>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="54"/>
-      <c r="S4" s="54"/>
-      <c r="T4" s="54"/>
-      <c r="U4" s="54"/>
-      <c r="V4" s="54"/>
-      <c r="W4" s="54"/>
-      <c r="X4" s="54"/>
-      <c r="Y4" s="54"/>
-      <c r="Z4" s="54"/>
-      <c r="AA4" s="54"/>
+      <c r="M4" s="67"/>
+      <c r="N4" s="67"/>
+      <c r="O4" s="67"/>
+      <c r="P4" s="67"/>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="67"/>
+      <c r="T4" s="67"/>
+      <c r="U4" s="67"/>
+      <c r="V4" s="67"/>
+      <c r="W4" s="67"/>
+      <c r="X4" s="67"/>
+      <c r="Y4" s="67"/>
+      <c r="Z4" s="67"/>
+      <c r="AA4" s="67"/>
     </row>
     <row r="5" spans="2:27" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="35" t="s">
@@ -48674,44 +48688,44 @@
       </c>
     </row>
     <row r="12" spans="2:5" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="55" t="s">
+      <c r="B12" s="54" t="s">
         <v>563</v>
       </c>
-      <c r="C12" s="56" t="s">
+      <c r="C12" s="55" t="s">
         <v>564</v>
       </c>
-      <c r="D12" s="57" t="s">
+      <c r="D12" s="56" t="s">
         <v>565</v>
       </c>
-      <c r="E12" s="57" t="s">
+      <c r="E12" s="56" t="s">
         <v>566</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="57" t="s">
         <v>551</v>
       </c>
       <c r="C13" s="28" t="s">
         <v>554</v>
       </c>
-      <c r="D13" s="59" t="s">
+      <c r="D13" s="58" t="s">
         <v>567</v>
       </c>
-      <c r="E13" s="60" t="s">
+      <c r="E13" s="59" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="57" t="s">
         <v>37</v>
       </c>
       <c r="C14" s="28" t="s">
         <v>554</v>
       </c>
-      <c r="D14" s="59" t="s">
+      <c r="D14" s="58" t="s">
         <v>567</v>
       </c>
-      <c r="E14" s="60" t="s">
+      <c r="E14" s="59" t="s">
         <v>569</v>
       </c>
     </row>
@@ -48722,10 +48736,10 @@
       <c r="C15" s="28" t="s">
         <v>570</v>
       </c>
-      <c r="D15" s="61" t="s">
+      <c r="D15" s="60" t="s">
         <v>523</v>
       </c>
-      <c r="E15" s="60" t="s">
+      <c r="E15" s="59" t="s">
         <v>571</v>
       </c>
     </row>
@@ -48919,7 +48933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D6B83C-E8B8-4DA4-8E51-8D3B78A1B9E1}">
   <dimension ref="B1:J169"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
@@ -48964,168 +48978,168 @@
       <c r="B7" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="66" t="s">
+      <c r="C7" s="65" t="s">
         <v>577</v>
       </c>
-      <c r="D7" s="66" t="s">
+      <c r="D7" s="65" t="s">
         <v>578</v>
       </c>
-      <c r="E7" s="66" t="s">
+      <c r="E7" s="65" t="s">
         <v>579</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="64">
+      <c r="C8" s="63">
         <v>177</v>
       </c>
-      <c r="D8" s="65">
-        <f>C8/$C$16</f>
+      <c r="D8" s="64">
+        <f t="shared" ref="D8:D15" si="0">C8/$C$16</f>
         <v>0.90769230769230769</v>
       </c>
-      <c r="E8" s="67">
+      <c r="E8" s="66">
         <f>D8</f>
         <v>0.90769230769230769</v>
       </c>
       <c r="J8" s="31"/>
     </row>
     <row r="9" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="64">
+      <c r="C9" s="63">
         <v>7</v>
       </c>
-      <c r="D9" s="65">
-        <f>C9/$C$16</f>
+      <c r="D9" s="64">
+        <f t="shared" si="0"/>
         <v>3.5897435897435895E-2</v>
       </c>
-      <c r="E9" s="67">
+      <c r="E9" s="66">
         <f>E8+D9</f>
         <v>0.94358974358974357</v>
       </c>
       <c r="J9" s="31"/>
     </row>
     <row r="10" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="64">
+      <c r="C10" s="63">
         <v>4</v>
       </c>
-      <c r="D10" s="65">
-        <f>C10/$C$16</f>
+      <c r="D10" s="64">
+        <f t="shared" si="0"/>
         <v>2.0512820512820513E-2</v>
       </c>
-      <c r="E10" s="67">
-        <f t="shared" ref="E10:E15" si="0">E9+D10</f>
+      <c r="E10" s="66">
+        <f t="shared" ref="E10:E15" si="1">E9+D10</f>
         <v>0.96410256410256412</v>
       </c>
       <c r="J10" s="31"/>
     </row>
     <row r="11" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="64">
+      <c r="C11" s="63">
         <v>2</v>
       </c>
-      <c r="D11" s="65">
-        <f>C11/$C$16</f>
+      <c r="D11" s="64">
+        <f t="shared" si="0"/>
         <v>1.0256410256410256E-2</v>
       </c>
-      <c r="E11" s="67">
+      <c r="E11" s="66">
+        <f t="shared" si="1"/>
+        <v>0.97435897435897434</v>
+      </c>
+      <c r="J11" s="31"/>
+    </row>
+    <row r="12" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B12" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="63">
+        <v>2</v>
+      </c>
+      <c r="D12" s="64">
         <f t="shared" si="0"/>
-        <v>0.97435897435897434</v>
-      </c>
-      <c r="J11" s="31"/>
-    </row>
-    <row r="12" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" s="63" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="64">
-        <v>2</v>
-      </c>
-      <c r="D12" s="65">
-        <f>C12/$C$16</f>
         <v>1.0256410256410256E-2</v>
       </c>
-      <c r="E12" s="67">
+      <c r="E12" s="66">
+        <f t="shared" si="1"/>
+        <v>0.98461538461538456</v>
+      </c>
+      <c r="J12" s="31"/>
+    </row>
+    <row r="13" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="63">
+        <v>1</v>
+      </c>
+      <c r="D13" s="64">
         <f t="shared" si="0"/>
-        <v>0.98461538461538456</v>
-      </c>
-      <c r="J12" s="31"/>
-    </row>
-    <row r="13" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="63" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="64">
+        <v>5.1282051282051282E-3</v>
+      </c>
+      <c r="E13" s="66">
+        <f t="shared" si="1"/>
+        <v>0.98974358974358967</v>
+      </c>
+      <c r="J13" s="31"/>
+    </row>
+    <row r="14" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B14" s="62" t="s">
+        <v>490</v>
+      </c>
+      <c r="C14" s="63">
         <v>1</v>
       </c>
-      <c r="D13" s="65">
-        <f>C13/$C$16</f>
+      <c r="D14" s="64">
+        <f t="shared" si="0"/>
         <v>5.1282051282051282E-3</v>
       </c>
-      <c r="E13" s="67">
+      <c r="E14" s="66">
+        <f t="shared" si="1"/>
+        <v>0.99487179487179478</v>
+      </c>
+      <c r="J14" s="31"/>
+    </row>
+    <row r="15" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B15" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="63">
+        <v>1</v>
+      </c>
+      <c r="D15" s="64">
         <f t="shared" si="0"/>
-        <v>0.98974358974358967</v>
-      </c>
-      <c r="J13" s="31"/>
-    </row>
-    <row r="14" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="63" t="s">
-        <v>490</v>
-      </c>
-      <c r="C14" s="64">
-        <v>1</v>
-      </c>
-      <c r="D14" s="65">
-        <f>C14/$C$16</f>
         <v>5.1282051282051282E-3</v>
       </c>
-      <c r="E14" s="67">
-        <f t="shared" si="0"/>
-        <v>0.99487179487179478</v>
-      </c>
-      <c r="J14" s="31"/>
-    </row>
-    <row r="15" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B15" s="63" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="64">
-        <v>1</v>
-      </c>
-      <c r="D15" s="65">
-        <f>C15/$C$16</f>
-        <v>5.1282051282051282E-3</v>
-      </c>
-      <c r="E15" s="67">
-        <f t="shared" si="0"/>
+      <c r="E15" s="66">
+        <f t="shared" si="1"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="J15" s="31"/>
     </row>
     <row r="16" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B16" s="63" t="s">
+      <c r="B16" s="62" t="s">
         <v>576</v>
       </c>
-      <c r="C16" s="64">
+      <c r="C16" s="63">
         <f>SUM(C8:C15)</f>
         <v>195</v>
       </c>
-      <c r="D16" s="65">
+      <c r="D16" s="64">
         <f>SUM(D8:D15)</f>
         <v>0.99999999999999989</v>
       </c>
       <c r="J16" s="31"/>
     </row>
     <row r="17" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="63"/>
+      <c r="B17" s="62"/>
       <c r="J17" s="31"/>
     </row>
     <row r="18" spans="2:10" ht="15" x14ac:dyDescent="0.25">
@@ -49601,15 +49615,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:X189"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2" style="32" customWidth="1"/>
-    <col min="2" max="2" width="7" style="32" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="32" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="32" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" style="32" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.85546875" style="32"/>
   </cols>
@@ -49707,21 +49721,63 @@
       <c r="H7" s="31"/>
     </row>
     <row r="8" spans="2:24" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" s="32" t="s">
+        <v>580</v>
+      </c>
+      <c r="C8" s="52">
+        <f>AVERAGE('365RE'!$I$6:$I$272)</f>
+        <v>281171.90150112362</v>
+      </c>
       <c r="H8" s="31"/>
     </row>
     <row r="9" spans="2:24" ht="15" x14ac:dyDescent="0.25">
+      <c r="B9" s="32" t="s">
+        <v>581</v>
+      </c>
+      <c r="C9" s="52">
+        <f>MEDIAN('365RE'!$I$6:$I$272)</f>
+        <v>249075.6568</v>
+      </c>
       <c r="H9" s="31"/>
     </row>
     <row r="10" spans="2:24" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" s="32" t="s">
+        <v>582</v>
+      </c>
+      <c r="C10" s="52">
+        <f>_xlfn.MODE.SNGL('365RE'!$I$6:$I$272)</f>
+        <v>460001.25599999994</v>
+      </c>
       <c r="H10" s="31"/>
     </row>
     <row r="11" spans="2:24" ht="15" x14ac:dyDescent="0.25">
+      <c r="B11" s="32" t="s">
+        <v>583</v>
+      </c>
+      <c r="C11" s="52">
+        <f>SKEW('365RE'!$I$6:$I$272)</f>
+        <v>1.0960149435317852</v>
+      </c>
       <c r="H11" s="31"/>
     </row>
     <row r="12" spans="2:24" ht="15" x14ac:dyDescent="0.25">
+      <c r="B12" s="32" t="s">
+        <v>584</v>
+      </c>
+      <c r="C12" s="52">
+        <f>_xlfn.VAR.S('365RE'!$I$6:$I$272)</f>
+        <v>7942217700.9209938</v>
+      </c>
       <c r="H12" s="31"/>
     </row>
     <row r="13" spans="2:24" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" s="32" t="s">
+        <v>585</v>
+      </c>
+      <c r="C13" s="52">
+        <f>_xlfn.STDEV.S('365RE'!$I$6:$I$272)</f>
+        <v>89119.120849125262</v>
+      </c>
       <c r="H13" s="31"/>
     </row>
     <row r="14" spans="2:24" ht="15" x14ac:dyDescent="0.25">
@@ -49731,6 +49787,9 @@
       <c r="H15" s="31"/>
     </row>
     <row r="16" spans="2:24" ht="15" x14ac:dyDescent="0.25">
+      <c r="B16" s="59" t="s">
+        <v>586</v>
+      </c>
       <c r="H16" s="31"/>
     </row>
     <row r="17" spans="8:8" ht="15" x14ac:dyDescent="0.25">
@@ -50326,7 +50385,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="61" t="s">
         <v>572</v>
       </c>
       <c r="B3" t="s">
@@ -50334,80 +50393,80 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="64">
+      <c r="B4" s="63">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="62" t="s">
         <v>490</v>
       </c>
-      <c r="B5" s="64">
+      <c r="B5" s="63">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="64">
+      <c r="B6" s="63">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="64">
+      <c r="B7" s="63">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="64">
+      <c r="B8" s="63">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="64">
+      <c r="B9" s="63">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="63" t="s">
+      <c r="A10" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="64">
+      <c r="B10" s="63">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="63" t="s">
+      <c r="A11" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="64">
+      <c r="B11" s="63">
         <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="63" t="s">
+      <c r="A12" s="62" t="s">
         <v>573</v>
       </c>
-      <c r="B12" s="64"/>
+      <c r="B12" s="63"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="62" t="s">
         <v>574</v>
       </c>
-      <c r="B13" s="64">
+      <c r="B13" s="63">
         <v>195</v>
       </c>
     </row>

</xml_diff>

<commit_message>
descriptive statistics q 10
</commit_message>
<xml_diff>
--- a/03-descriptive statistics/descriptive-statistics.xlsx
+++ b/03-descriptive statistics/descriptive-statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\statistics-4-data-science-business-analysis\03-descriptive statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728C0DC7-63B6-462A-86BB-38C46B74AA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A4CF7E-C93E-4902-9414-BD609F9B937D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="365RE" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="Tasks 6,7" sheetId="10" r:id="rId5"/>
     <sheet name="Tasks 8,9" sheetId="5" r:id="rId6"/>
     <sheet name="Task 10" sheetId="6" r:id="rId7"/>
-    <sheet name="customer by country" sheetId="13" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'365RE'!$A$5:$AM$926</definedName>
@@ -32,9 +31,6 @@
     <definedName name="_xlchart.v1.5" hidden="1">'Tasks 6,7'!$E$8:$E$15</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId9"/>
-  </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -48,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2567" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2558" uniqueCount="586">
   <si>
     <t>Office</t>
   </si>
@@ -1903,18 +1899,6 @@
     <t>Year is a numerical variable. It is always discrete. The level of measurement is questionable, but we would treat it as interval, as the 0 year would be the time when the Big Bang happened. The current BC-AD calendar was arbitrary chosen (similarly to degrees Celsius and Fahrenheit).</t>
   </si>
   <si>
-    <t>Row Labels</t>
-  </si>
-  <si>
-    <t>(blank)</t>
-  </si>
-  <si>
-    <t>Grand Total</t>
-  </si>
-  <si>
-    <t>Count of Customer ID</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -1946,6 +1930,15 @@
   </si>
   <si>
     <t>We will only comment on the skew, as it is a bit tougher. The skew is right (positive). This means that most properties are relatively cheap with a tiny portion that is more expensive.</t>
+  </si>
+  <si>
+    <t>covariance</t>
+  </si>
+  <si>
+    <t>correlation coefficient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, the result is in line with the scatter plot. The two variables are greatly correlated. </t>
   </si>
 </sst>
 </file>
@@ -2117,7 +2110,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2275,7 +2268,6 @@
     <xf numFmtId="9" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -7030,3699 +7022,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="STC" refreshedDate="44844.419149305555" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="196" xr:uid="{BA9B01C4-1C6A-4C6C-A1CF-CAFB8F1BD9B7}">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="L5:AA201" sheet="365RE"/>
-  </cacheSource>
-  <cacheFields count="16">
-    <cacheField name="Customer ID" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Entity" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Name" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Surname" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Age at time of purchase" numFmtId="0">
-      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="19" maxValue="76"/>
-    </cacheField>
-    <cacheField name="Interval" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Y" numFmtId="0">
-      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1931" maxValue="1986"/>
-    </cacheField>
-    <cacheField name="M" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1" maxValue="15"/>
-    </cacheField>
-    <cacheField name="D" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1" maxValue="31"/>
-    </cacheField>
-    <cacheField name="Gender" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Country" numFmtId="0">
-      <sharedItems containsBlank="1" count="9">
-        <s v="USA"/>
-        <s v="UK"/>
-        <s v="Belgium"/>
-        <s v="Russia"/>
-        <s v="Denmark"/>
-        <s v="Germany"/>
-        <s v="Mexico"/>
-        <s v="Canada"/>
-        <m/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="State" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Purpose" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Deal satisfaction" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
-    </cacheField>
-    <cacheField name="Mortgage" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Source" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="196">
-  <r>
-    <s v="C0028"/>
-    <s v="Individual"/>
-    <s v="Madalyn"/>
-    <s v="Mercer"/>
-    <n v="19"/>
-    <s v="18-25"/>
-    <n v="1986"/>
-    <n v="6"/>
-    <n v="21"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0027"/>
-    <s v="Individual"/>
-    <s v="Lara"/>
-    <s v="Carrillo"/>
-    <n v="22"/>
-    <s v="18-25"/>
-    <n v="1983"/>
-    <n v="2"/>
-    <n v="23.999999999999996"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0112"/>
-    <s v="Individual"/>
-    <s v="Donavan"/>
-    <s v="Flowers"/>
-    <n v="22"/>
-    <s v="18-25"/>
-    <n v="1985"/>
-    <n v="12"/>
-    <n v="27"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="1"/>
-    <s v="Yes"/>
-    <s v="Client"/>
-  </r>
-  <r>
-    <s v="C0160"/>
-    <s v="Individual"/>
-    <s v="Darien"/>
-    <s v="Dorsey"/>
-    <n v="22"/>
-    <s v="18-25"/>
-    <n v="1985"/>
-    <n v="12"/>
-    <n v="27"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="3"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0014"/>
-    <s v="Individual"/>
-    <s v="Alessandra"/>
-    <s v="Perry"/>
-    <n v="25"/>
-    <s v="18-25"/>
-    <n v="1979"/>
-    <n v="5"/>
-    <n v="15"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0125"/>
-    <s v="Individual"/>
-    <s v="Kaitlin"/>
-    <s v="Owen"/>
-    <n v="26"/>
-    <s v="26-35"/>
-    <n v="1981"/>
-    <n v="12"/>
-    <n v="26"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="Virginia"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Client"/>
-  </r>
-  <r>
-    <s v="C0125"/>
-    <s v="Individual"/>
-    <s v="Kaitlin"/>
-    <s v="Owen"/>
-    <n v="26"/>
-    <s v="26-35"/>
-    <n v="1981"/>
-    <n v="12"/>
-    <n v="26"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="Virginia"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0166"/>
-    <s v="Individual"/>
-    <s v="Terry"/>
-    <s v="Forbes"/>
-    <n v="26"/>
-    <s v="26-35"/>
-    <n v="1982"/>
-    <n v="5"/>
-    <n v="27"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Client"/>
-  </r>
-  <r>
-    <s v="C0034"/>
-    <s v="Individual"/>
-    <s v="Kole"/>
-    <s v="Shannon"/>
-    <n v="27"/>
-    <s v="26-35"/>
-    <n v="1979"/>
-    <n v="6"/>
-    <n v="27"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Arizona"/>
-    <s v="Home"/>
-    <n v="2"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0170"/>
-    <s v="Individual"/>
-    <s v="Emmy"/>
-    <s v="Singh"/>
-    <n v="27"/>
-    <s v="26-35"/>
-    <n v="1979"/>
-    <n v="12"/>
-    <n v="3"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="Virginia"/>
-    <s v="Investment"/>
-    <n v="3"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0009"/>
-    <s v="Individual"/>
-    <s v="Arabella"/>
-    <s v="Ferrell"/>
-    <n v="28"/>
-    <s v="26-35"/>
-    <n v="1976"/>
-    <n v="8"/>
-    <n v="17"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="Oregon"/>
-    <s v="Home"/>
-    <n v="1"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0041"/>
-    <s v="Individual"/>
-    <s v="Christian"/>
-    <s v="Costa"/>
-    <n v="26"/>
-    <s v="26-35"/>
-    <n v="1980"/>
-    <n v="9"/>
-    <n v="14"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0057"/>
-    <s v="Individual"/>
-    <s v="Michelle"/>
-    <s v="Cameron"/>
-    <n v="29"/>
-    <s v="26-35"/>
-    <n v="1978"/>
-    <n v="6"/>
-    <n v="4"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="Nevada"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0061"/>
-    <s v="Individual"/>
-    <s v="Enrique"/>
-    <s v="Cardenas"/>
-    <n v="29"/>
-    <s v="26-35"/>
-    <n v="1977"/>
-    <n v="6"/>
-    <n v="10"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="2"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0089"/>
-    <s v="Individual"/>
-    <s v="Amanda"/>
-    <s v="Simon"/>
-    <n v="29"/>
-    <s v="26-35"/>
-    <n v="1978"/>
-    <n v="12"/>
-    <n v="2.9999999999999996"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0159"/>
-    <s v="Individual"/>
-    <s v="Kamden"/>
-    <s v="Stewart"/>
-    <n v="29"/>
-    <s v="26-35"/>
-    <n v="1978"/>
-    <n v="9"/>
-    <n v="14"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0171"/>
-    <s v="Individual"/>
-    <s v="Skylar"/>
-    <s v="Buchanan"/>
-    <n v="29"/>
-    <s v="26-35"/>
-    <n v="1977"/>
-    <n v="12"/>
-    <n v="25"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Nevada"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0042"/>
-    <s v="Individual"/>
-    <s v="Michael"/>
-    <s v="Juarez"/>
-    <n v="30"/>
-    <s v="26-35"/>
-    <n v="1976"/>
-    <n v="12"/>
-    <n v="25"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Colorado"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0093"/>
-    <s v="Individual"/>
-    <s v="Antonio"/>
-    <s v="Porter"/>
-    <n v="30"/>
-    <s v="26-35"/>
-    <n v="1977"/>
-    <n v="1"/>
-    <n v="8"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Arizona"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Client"/>
-  </r>
-  <r>
-    <s v="C0093"/>
-    <s v="Individual"/>
-    <s v="Antonio"/>
-    <s v="Porter"/>
-    <n v="30"/>
-    <s v="26-35"/>
-    <n v="1977"/>
-    <n v="1"/>
-    <n v="8"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Arizona"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Client"/>
-  </r>
-  <r>
-    <s v="C0051"/>
-    <s v="Individual"/>
-    <s v="Conner"/>
-    <s v="Huff"/>
-    <n v="31"/>
-    <s v="26-35"/>
-    <n v="1975"/>
-    <n v="3"/>
-    <n v="22"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Nevada"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0064"/>
-    <s v="Individual"/>
-    <s v="Joaquin"/>
-    <s v="Mullins"/>
-    <n v="31"/>
-    <s v="26-35"/>
-    <n v="1975"/>
-    <n v="10"/>
-    <n v="5"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0064"/>
-    <s v="Individual"/>
-    <s v="Joaquin"/>
-    <s v="Mullins"/>
-    <n v="31"/>
-    <s v="26-35"/>
-    <n v="1975"/>
-    <n v="10"/>
-    <n v="5"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0128"/>
-    <s v="Individual"/>
-    <s v="Kyla"/>
-    <s v="Walker"/>
-    <n v="31"/>
-    <s v="26-35"/>
-    <n v="1976"/>
-    <n v="2"/>
-    <n v="26"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="Colorado"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0019"/>
-    <s v="Individual"/>
-    <s v="Victor"/>
-    <s v="Jensen"/>
-    <n v="32"/>
-    <s v="26-35"/>
-    <n v="1973"/>
-    <n v="9"/>
-    <n v="1"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0037"/>
-    <s v="Individual"/>
-    <s v="Tyler"/>
-    <s v="Carr"/>
-    <n v="32"/>
-    <s v="26-35"/>
-    <n v="1974"/>
-    <n v="3"/>
-    <n v="27"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="Yes"/>
-    <s v="Client"/>
-  </r>
-  <r>
-    <s v="C0127"/>
-    <s v="Individual"/>
-    <s v="Maia"/>
-    <s v="Chandler"/>
-    <n v="32"/>
-    <s v="26-35"/>
-    <n v="1975"/>
-    <n v="8"/>
-    <n v="11.999999999999998"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="Utah"/>
-    <s v="Home"/>
-    <n v="1"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0018"/>
-    <s v="Individual"/>
-    <s v="Rodrigo"/>
-    <s v="Ramirez"/>
-    <n v="33"/>
-    <s v="26-35"/>
-    <n v="1972"/>
-    <n v="3"/>
-    <n v="26"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="1"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0040"/>
-    <s v="Individual"/>
-    <s v="Gianni"/>
-    <s v="Fritz"/>
-    <n v="33"/>
-    <s v="26-35"/>
-    <n v="1973"/>
-    <n v="9"/>
-    <n v="15"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0080"/>
-    <s v="Individual"/>
-    <s v="Janelle"/>
-    <s v="Espinoza"/>
-    <n v="33"/>
-    <s v="26-35"/>
-    <n v="1974"/>
-    <n v="12"/>
-    <n v="25"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Client"/>
-  </r>
-  <r>
-    <s v="C0083"/>
-    <s v="Individual"/>
-    <s v="Julio"/>
-    <s v="Leonard"/>
-    <n v="33"/>
-    <s v="26-35"/>
-    <n v="1974"/>
-    <n v="7.0000000000000009"/>
-    <n v="18"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Nevada"/>
-    <s v="Home"/>
-    <n v="2"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0085"/>
-    <s v="Individual"/>
-    <s v="Melanie"/>
-    <s v="Holland"/>
-    <n v="33"/>
-    <s v="26-35"/>
-    <n v="1974"/>
-    <n v="12"/>
-    <n v="25"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Client"/>
-  </r>
-  <r>
-    <s v="C0091"/>
-    <s v="Individual"/>
-    <s v="Gordon"/>
-    <s v="Brown"/>
-    <n v="33"/>
-    <s v="26-35"/>
-    <n v="1974"/>
-    <n v="2"/>
-    <n v="10"/>
-    <s v="M"/>
-    <x v="1"/>
-    <s v="Arizona"/>
-    <s v="Investment"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0007"/>
-    <s v="Individual"/>
-    <s v="Jaelyn"/>
-    <s v="Berger"/>
-    <n v="34"/>
-    <s v="26-35"/>
-    <n v="1970"/>
-    <n v="5"/>
-    <n v="5"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0048"/>
-    <s v="Individual"/>
-    <s v="Adriana"/>
-    <s v="Shaffer"/>
-    <n v="34"/>
-    <s v="26-35"/>
-    <n v="1972"/>
-    <n v="7.0000000000000009"/>
-    <n v="11"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="2"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0065"/>
-    <s v="Individual"/>
-    <s v="Mara"/>
-    <s v="Franco"/>
-    <n v="34"/>
-    <s v="26-35"/>
-    <n v="1973"/>
-    <n v="6"/>
-    <n v="7"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0096"/>
-    <s v="Individual"/>
-    <s v="Kael"/>
-    <s v="Hurley"/>
-    <n v="34"/>
-    <s v="26-35"/>
-    <n v="1973"/>
-    <n v="12"/>
-    <n v="15"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Colorado"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0164"/>
-    <s v="Individual"/>
-    <s v="Belinda"/>
-    <s v="Hogan"/>
-    <n v="34"/>
-    <s v="26-35"/>
-    <n v="1973"/>
-    <n v="8"/>
-    <n v="18"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="1"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0038"/>
-    <s v="Individual"/>
-    <s v="Mohammad"/>
-    <s v="Irwin"/>
-    <n v="35"/>
-    <s v="26-35"/>
-    <n v="1971"/>
-    <n v="12"/>
-    <n v="2"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="1"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0087"/>
-    <s v="Individual"/>
-    <s v="Warren"/>
-    <s v="Pugh"/>
-    <n v="35"/>
-    <s v="26-35"/>
-    <n v="1973"/>
-    <n v="7"/>
-    <n v="17"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Arizona"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0142"/>
-    <s v="Individual"/>
-    <s v="Kassidy"/>
-    <s v="Vega"/>
-    <n v="35"/>
-    <s v="26-35"/>
-    <n v="1972"/>
-    <n v="5"/>
-    <n v="7"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0015"/>
-    <s v="Individual"/>
-    <s v="Lauryn"/>
-    <s v="Patrick"/>
-    <n v="36"/>
-    <s v="36-45"/>
-    <n v="1969"/>
-    <n v="10"/>
-    <n v="30"/>
-    <s v="F"/>
-    <x v="2"/>
-    <m/>
-    <s v="Home"/>
-    <n v="2"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0122"/>
-    <s v="Individual"/>
-    <s v="Brock"/>
-    <s v="Fischer"/>
-    <n v="36"/>
-    <s v="36-45"/>
-    <n v="1971"/>
-    <n v="5"/>
-    <n v="28.999999999999996"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Kansas"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0017"/>
-    <s v="Individual"/>
-    <s v="Memphis"/>
-    <s v="Mcconnell"/>
-    <n v="37"/>
-    <s v="36-45"/>
-    <n v="1968"/>
-    <n v="8"/>
-    <n v="25"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="2"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0020"/>
-    <s v="Individual"/>
-    <s v="Grant"/>
-    <s v="Weber"/>
-    <n v="37"/>
-    <s v="36-45"/>
-    <n v="1968"/>
-    <n v="9"/>
-    <n v="8"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0086"/>
-    <s v="Individual"/>
-    <s v="Jace"/>
-    <s v="Riggs"/>
-    <n v="37"/>
-    <s v="36-45"/>
-    <n v="1971"/>
-    <n v="8"/>
-    <n v="20"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="1"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0150"/>
-    <s v="Individual"/>
-    <s v="Emmett"/>
-    <s v="Estes"/>
-    <n v="37"/>
-    <s v="36-45"/>
-    <n v="1969"/>
-    <n v="6"/>
-    <n v="5"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0156"/>
-    <s v="Individual"/>
-    <s v="Isis"/>
-    <s v="Rios"/>
-    <n v="37"/>
-    <s v="36-45"/>
-    <n v="1970"/>
-    <n v="4"/>
-    <n v="1"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0169"/>
-    <s v="Individual"/>
-    <s v="Mason"/>
-    <s v="Gilbert"/>
-    <n v="37"/>
-    <s v="36-45"/>
-    <n v="1970"/>
-    <n v="7"/>
-    <n v="31"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Colorado"/>
-    <s v="Home"/>
-    <n v="2"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0022"/>
-    <s v="Individual"/>
-    <s v="Zain"/>
-    <s v="Horne"/>
-    <n v="38"/>
-    <s v="36-45"/>
-    <n v="1967"/>
-    <n v="4"/>
-    <n v="13"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Arizona"/>
-    <s v="Home"/>
-    <n v="1"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0072"/>
-    <s v="Individual"/>
-    <s v="Dayton"/>
-    <s v="Hatfield"/>
-    <n v="38"/>
-    <s v="36-45"/>
-    <n v="1969"/>
-    <n v="4"/>
-    <n v="19"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Colorado"/>
-    <s v="Investment"/>
-    <n v="4"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0136"/>
-    <s v="Individual"/>
-    <s v="Annabel"/>
-    <s v="Robles"/>
-    <n v="38"/>
-    <s v="36-45"/>
-    <n v="1969"/>
-    <n v="10"/>
-    <n v="14"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0149"/>
-    <s v="Individual"/>
-    <s v="Kayden"/>
-    <s v="Olsen"/>
-    <n v="38"/>
-    <s v="36-45"/>
-    <n v="1969"/>
-    <n v="10"/>
-    <n v="17"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0011"/>
-    <s v="Individual"/>
-    <s v="Davion"/>
-    <s v="Stout"/>
-    <n v="39"/>
-    <s v="36-45"/>
-    <n v="1965"/>
-    <n v="7.0000000000000009"/>
-    <n v="20"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Nevada"/>
-    <s v="Home"/>
-    <n v="1"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0073"/>
-    <s v="Individual"/>
-    <s v="Kevin"/>
-    <s v="Mata"/>
-    <n v="39"/>
-    <s v="36-45"/>
-    <n v="1968"/>
-    <n v="10"/>
-    <n v="11.999999999999998"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Colorado"/>
-    <s v="Investment"/>
-    <n v="2"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0110"/>
-    <s v="Individual"/>
-    <s v="Kareem"/>
-    <s v="Liu"/>
-    <n v="39"/>
-    <s v="36-45"/>
-    <n v="1968"/>
-    <n v="5"/>
-    <n v="11"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0111"/>
-    <s v="Individual"/>
-    <s v="Grace"/>
-    <s v="Stein"/>
-    <n v="39"/>
-    <s v="36-45"/>
-    <n v="1968"/>
-    <n v="12"/>
-    <n v="20"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0123"/>
-    <s v="Individual"/>
-    <s v="Lydia"/>
-    <s v="Tate"/>
-    <n v="39"/>
-    <s v="36-45"/>
-    <n v="1968"/>
-    <n v="8"/>
-    <n v="14"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0070"/>
-    <s v="Individual"/>
-    <s v="Aleksandra"/>
-    <s v="Karenina"/>
-    <n v="40"/>
-    <s v="36-45"/>
-    <n v="1967"/>
-    <n v="6"/>
-    <n v="13"/>
-    <s v="F"/>
-    <x v="3"/>
-    <m/>
-    <s v="Home"/>
-    <n v="1"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0075"/>
-    <s v="Individual"/>
-    <s v="Sincere"/>
-    <s v="Hansen"/>
-    <n v="40"/>
-    <s v="36-45"/>
-    <n v="1967"/>
-    <n v="1"/>
-    <n v="19"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="2"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0076"/>
-    <s v="Individual"/>
-    <s v="Luke"/>
-    <s v="Lynn"/>
-    <n v="40"/>
-    <s v="36-45"/>
-    <n v="1967"/>
-    <n v="2"/>
-    <n v="7"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="2"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0105"/>
-    <s v="Individual"/>
-    <s v="Myla"/>
-    <s v="Ewing"/>
-    <n v="40"/>
-    <s v="36-45"/>
-    <n v="1967"/>
-    <n v="2"/>
-    <n v="2.9999999999999996"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="Oregon"/>
-    <s v="Investment"/>
-    <n v="2"/>
-    <s v="No"/>
-    <s v="Client"/>
-  </r>
-  <r>
-    <s v="C0135"/>
-    <s v="Individual"/>
-    <s v="Morgan"/>
-    <s v="Glass"/>
-    <n v="40"/>
-    <s v="36-45"/>
-    <n v="1967"/>
-    <n v="5"/>
-    <n v="11.999999999999998"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Utah"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0153"/>
-    <s v="Individual"/>
-    <s v="Camille"/>
-    <s v="Sharp"/>
-    <n v="40"/>
-    <s v="36-45"/>
-    <n v="1967"/>
-    <n v="10"/>
-    <n v="17"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0047"/>
-    <s v="Individual"/>
-    <s v="Alejandra"/>
-    <s v="Greer"/>
-    <n v="41"/>
-    <s v="36-45"/>
-    <n v="1965"/>
-    <n v="1"/>
-    <n v="11"/>
-    <s v="F"/>
-    <x v="4"/>
-    <m/>
-    <s v="Investment"/>
-    <n v="1"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0060"/>
-    <s v="Individual"/>
-    <s v="Valentina"/>
-    <s v="Simpson"/>
-    <n v="41"/>
-    <s v="36-45"/>
-    <n v="1965"/>
-    <n v="1"/>
-    <n v="23.999999999999996"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0066"/>
-    <s v="Individual"/>
-    <s v="Helen"/>
-    <s v="Williamson"/>
-    <n v="41"/>
-    <s v="36-45"/>
-    <n v="1966"/>
-    <n v="2"/>
-    <n v="26"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="Colorado"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0068"/>
-    <s v="Individual"/>
-    <s v="Nicolas"/>
-    <s v="Navarro"/>
-    <n v="41"/>
-    <s v="36-45"/>
-    <n v="1966"/>
-    <n v="6"/>
-    <n v="17"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Oregon"/>
-    <s v="Investment"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0090"/>
-    <s v="Individual"/>
-    <s v="Case"/>
-    <s v="Sanchez"/>
-    <n v="41"/>
-    <s v="36-45"/>
-    <n v="1966"/>
-    <n v="5"/>
-    <n v="26"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0095"/>
-    <s v="Individual"/>
-    <s v="Rodrigo"/>
-    <s v="Robinson"/>
-    <n v="41"/>
-    <s v="36-45"/>
-    <n v="1966"/>
-    <n v="8"/>
-    <n v="11"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0151"/>
-    <s v="Individual"/>
-    <s v="Iris"/>
-    <s v="Larsen"/>
-    <n v="41"/>
-    <s v="36-45"/>
-    <n v="1966"/>
-    <n v="9"/>
-    <n v="14"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0162"/>
-    <s v="Individual"/>
-    <s v="Araceli"/>
-    <s v="Nelson"/>
-    <n v="41"/>
-    <s v="36-45"/>
-    <n v="1966"/>
-    <n v="9"/>
-    <n v="14"/>
-    <s v="M"/>
-    <x v="5"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0010"/>
-    <s v="Individual"/>
-    <s v="Trystan"/>
-    <s v="Oconnor"/>
-    <n v="42"/>
-    <s v="36-45"/>
-    <n v="1962"/>
-    <n v="11"/>
-    <n v="26"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="1"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0054"/>
-    <s v="Individual"/>
-    <s v="Erik"/>
-    <s v="Mora"/>
-    <n v="42"/>
-    <s v="36-45"/>
-    <n v="1964"/>
-    <n v="12"/>
-    <n v="7"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Oregon"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0056"/>
-    <s v="Individual"/>
-    <s v="Emely"/>
-    <s v="Watts"/>
-    <n v="42"/>
-    <s v="36-45"/>
-    <n v="1964"/>
-    <n v="11"/>
-    <n v="30"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0081"/>
-    <s v="Individual"/>
-    <s v="Jordyn"/>
-    <s v="Park"/>
-    <n v="42"/>
-    <s v="36-45"/>
-    <n v="1965"/>
-    <n v="4"/>
-    <n v="4"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Nevada"/>
-    <s v="Investment"/>
-    <n v="3"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0084"/>
-    <s v="Individual"/>
-    <s v="Diego"/>
-    <s v="Mendez"/>
-    <n v="42"/>
-    <s v="36-45"/>
-    <n v="1965"/>
-    <n v="5"/>
-    <n v="12"/>
-    <s v="M"/>
-    <x v="6"/>
-    <m/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0016"/>
-    <s v="Individual"/>
-    <s v="Harley"/>
-    <s v="Lucero"/>
-    <n v="43"/>
-    <s v="36-45"/>
-    <n v="1962"/>
-    <n v="8"/>
-    <n v="10"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="1"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0035"/>
-    <s v="Individual"/>
-    <s v="Emilie"/>
-    <s v="Morrison"/>
-    <n v="49"/>
-    <s v="46-55"/>
-    <n v="1957"/>
-    <n v="10"/>
-    <n v="28.999999999999996"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0062"/>
-    <s v="Individual"/>
-    <s v="Jaylen"/>
-    <s v="Turner"/>
-    <n v="43"/>
-    <s v="36-45"/>
-    <n v="1963"/>
-    <n v="7.0000000000000009"/>
-    <n v="15"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0099"/>
-    <s v="Individual"/>
-    <s v="Frank"/>
-    <s v="Meyer"/>
-    <n v="43"/>
-    <s v="36-45"/>
-    <n v="1964"/>
-    <n v="3"/>
-    <n v="16"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="2"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0099"/>
-    <s v="Individual"/>
-    <s v="Frank"/>
-    <s v="Meyer"/>
-    <n v="43"/>
-    <s v="36-45"/>
-    <n v="1964"/>
-    <n v="3"/>
-    <n v="16"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0114"/>
-    <s v="Individual"/>
-    <s v="Jakobe"/>
-    <s v="Bailey"/>
-    <n v="43"/>
-    <s v="36-45"/>
-    <n v="1964"/>
-    <n v="10"/>
-    <n v="5.9999999999999991"/>
-    <s v="M"/>
-    <x v="1"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0006"/>
-    <s v="Individual"/>
-    <s v="Laci"/>
-    <s v="Guerra"/>
-    <n v="48"/>
-    <s v="46-55"/>
-    <n v="1956"/>
-    <n v="6"/>
-    <n v="17"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="2"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0053"/>
-    <s v="Individual"/>
-    <s v="Scarlet"/>
-    <s v="Hendricks"/>
-    <n v="44"/>
-    <s v="36-45"/>
-    <n v="1962"/>
-    <n v="1"/>
-    <n v="20"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0069"/>
-    <s v="Individual"/>
-    <s v="Alonso"/>
-    <s v="Terrell"/>
-    <n v="44"/>
-    <s v="36-45"/>
-    <n v="1963"/>
-    <n v="11"/>
-    <n v="5"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0069"/>
-    <s v="Individual"/>
-    <s v="Alonso"/>
-    <s v="Terrell"/>
-    <n v="44"/>
-    <s v="36-45"/>
-    <n v="1963"/>
-    <n v="11"/>
-    <n v="5"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0069"/>
-    <s v="Individual"/>
-    <s v="Alonso"/>
-    <s v="Terrell"/>
-    <n v="44"/>
-    <s v="36-45"/>
-    <n v="1963"/>
-    <n v="11"/>
-    <n v="5"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0077"/>
-    <s v="Individual"/>
-    <s v="Hazel"/>
-    <s v="Ayers"/>
-    <n v="44"/>
-    <s v="36-45"/>
-    <n v="1963"/>
-    <n v="2"/>
-    <n v="1"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Colorado"/>
-    <s v="Home"/>
-    <n v="2"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0168"/>
-    <s v="Individual"/>
-    <s v="Brisa"/>
-    <s v="Mckee"/>
-    <n v="44"/>
-    <s v="36-45"/>
-    <n v="1964"/>
-    <n v="9"/>
-    <n v="24"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Client"/>
-  </r>
-  <r>
-    <s v="C0058"/>
-    <s v="Individual"/>
-    <s v="Johanna"/>
-    <s v="Fisher"/>
-    <n v="45"/>
-    <s v="36-45"/>
-    <n v="1962"/>
-    <n v="8"/>
-    <n v="25"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0107"/>
-    <s v="Individual"/>
-    <s v="Curtis"/>
-    <s v="Howard"/>
-    <n v="45"/>
-    <s v="36-45"/>
-    <n v="1962"/>
-    <n v="9"/>
-    <n v="11"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="2"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0131"/>
-    <s v="Individual"/>
-    <s v="Kamila"/>
-    <s v="Collier"/>
-    <n v="45"/>
-    <s v="36-45"/>
-    <n v="1962"/>
-    <n v="1"/>
-    <n v="21"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="1"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0144"/>
-    <s v="Individual"/>
-    <s v="Joseph"/>
-    <s v="Reeves"/>
-    <n v="45"/>
-    <s v="36-45"/>
-    <n v="1962"/>
-    <n v="9"/>
-    <n v="23"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0144"/>
-    <s v="Individual"/>
-    <s v="Joseph"/>
-    <s v="Reeves"/>
-    <n v="45"/>
-    <s v="36-45"/>
-    <n v="1962"/>
-    <n v="9"/>
-    <n v="23"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0048"/>
-    <s v="Individual"/>
-    <s v="Adriana"/>
-    <s v="Shaffer"/>
-    <n v="47"/>
-    <s v="46-55"/>
-    <n v="1959"/>
-    <n v="9"/>
-    <n v="28"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="Utah"/>
-    <s v="Investment"/>
-    <n v="1"/>
-    <s v="No"/>
-    <s v="Client"/>
-  </r>
-  <r>
-    <s v="C0098"/>
-    <s v="Individual"/>
-    <s v="Oswaldo"/>
-    <s v="Palmer"/>
-    <n v="47"/>
-    <s v="46-55"/>
-    <n v="1960"/>
-    <n v="6"/>
-    <n v="16"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="2"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0130"/>
-    <s v="Individual"/>
-    <s v="Ezra"/>
-    <s v="Lozano"/>
-    <n v="47"/>
-    <s v="46-55"/>
-    <n v="1958"/>
-    <n v="2"/>
-    <n v="24"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="1"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0141"/>
-    <s v="Individual"/>
-    <s v="Melany"/>
-    <s v="Glover"/>
-    <n v="47"/>
-    <s v="46-55"/>
-    <n v="1960"/>
-    <n v="10"/>
-    <n v="1"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="1"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0067"/>
-    <s v="Individual"/>
-    <s v="Jacqueline"/>
-    <s v="Grant"/>
-    <n v="48"/>
-    <s v="46-55"/>
-    <n v="1959"/>
-    <n v="11"/>
-    <n v="13"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0082"/>
-    <s v="Individual"/>
-    <s v="Violet"/>
-    <s v="Nixon"/>
-    <n v="48"/>
-    <s v="46-55"/>
-    <n v="1959"/>
-    <n v="1"/>
-    <n v="1"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="Oregon"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Client"/>
-  </r>
-  <r>
-    <s v="C0113"/>
-    <s v="Individual"/>
-    <s v="Anya"/>
-    <s v="Stephenson"/>
-    <n v="48"/>
-    <s v="46-55"/>
-    <n v="1959"/>
-    <n v="6"/>
-    <n v="11"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0132"/>
-    <s v="Individual"/>
-    <s v="Kale"/>
-    <s v="Gay"/>
-    <n v="48"/>
-    <s v="46-55"/>
-    <n v="1959"/>
-    <n v="4"/>
-    <n v="7"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0137"/>
-    <s v="Individual"/>
-    <s v="Russell"/>
-    <s v="Gross"/>
-    <n v="48"/>
-    <s v="46-55"/>
-    <n v="1959"/>
-    <n v="11"/>
-    <n v="25"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0137"/>
-    <s v="Individual"/>
-    <s v="Russell"/>
-    <s v="Gross"/>
-    <n v="48"/>
-    <s v="46-55"/>
-    <n v="1959"/>
-    <n v="11"/>
-    <n v="25"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0155"/>
-    <s v="Individual"/>
-    <s v="Laurel"/>
-    <s v="Benitez"/>
-    <n v="48"/>
-    <s v="46-55"/>
-    <n v="1959"/>
-    <n v="8"/>
-    <n v="5.9999999999999991"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0163"/>
-    <s v="Individual"/>
-    <s v="Aniyah"/>
-    <s v="Ali"/>
-    <n v="48"/>
-    <s v="46-55"/>
-    <n v="1959"/>
-    <n v="11"/>
-    <n v="2.9999999999999996"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="2"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0039"/>
-    <s v="Individual"/>
-    <s v="Derick"/>
-    <s v="Li"/>
-    <n v="49"/>
-    <s v="46-55"/>
-    <n v="1957"/>
-    <n v="3"/>
-    <n v="20"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0071"/>
-    <s v="Individual"/>
-    <s v="Cole"/>
-    <s v="Taylor"/>
-    <n v="49"/>
-    <s v="46-55"/>
-    <n v="1958"/>
-    <n v="12"/>
-    <n v="5.9999999999999991"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0101"/>
-    <s v="Individual"/>
-    <s v="Ava"/>
-    <s v="Phelps"/>
-    <n v="49"/>
-    <s v="46-55"/>
-    <n v="1958"/>
-    <n v="4"/>
-    <n v="15"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Client"/>
-  </r>
-  <r>
-    <s v="C0146"/>
-    <s v="Individual"/>
-    <s v="Nyla"/>
-    <s v="Blake"/>
-    <n v="49"/>
-    <s v="46-55"/>
-    <n v="1959"/>
-    <n v="6"/>
-    <n v="5"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0051"/>
-    <s v="Individual"/>
-    <s v="Conner"/>
-    <s v="Huff"/>
-    <n v="50"/>
-    <s v="46-55"/>
-    <n v="1956"/>
-    <n v="3"/>
-    <n v="13"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0052"/>
-    <s v="Individual"/>
-    <s v="Tristian"/>
-    <s v="Fuller"/>
-    <n v="50"/>
-    <s v="46-55"/>
-    <n v="1956"/>
-    <n v="3"/>
-    <n v="13"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0052"/>
-    <s v="Individual"/>
-    <s v="Tristian"/>
-    <s v="Fuller"/>
-    <n v="50"/>
-    <s v="46-55"/>
-    <n v="1956"/>
-    <n v="3"/>
-    <n v="13"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0063"/>
-    <s v="Individual"/>
-    <s v="Piotr"/>
-    <s v="Aleksandrov"/>
-    <n v="51"/>
-    <s v="46-55"/>
-    <n v="1955"/>
-    <n v="12"/>
-    <n v="2"/>
-    <s v="M"/>
-    <x v="3"/>
-    <m/>
-    <s v="Investment"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0088"/>
-    <s v="Individual"/>
-    <s v="Yurem"/>
-    <s v="Wright"/>
-    <n v="51"/>
-    <s v="46-55"/>
-    <n v="1957"/>
-    <n v="3"/>
-    <n v="6"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0094"/>
-    <s v="Individual"/>
-    <s v="Luis"/>
-    <s v="Crane"/>
-    <n v="51"/>
-    <s v="46-55"/>
-    <n v="1959"/>
-    <n v="4"/>
-    <n v="20"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Nevada"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0165"/>
-    <s v="Individual"/>
-    <s v="Anahi"/>
-    <s v="Curry"/>
-    <n v="51"/>
-    <s v="46-55"/>
-    <n v="1957"/>
-    <n v="9"/>
-    <n v="9"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="Yes"/>
-    <s v="Client"/>
-  </r>
-  <r>
-    <s v="C0044"/>
-    <s v="Individual"/>
-    <s v="Ramiro"/>
-    <s v="Oneill"/>
-    <n v="52"/>
-    <s v="46-55"/>
-    <n v="1954"/>
-    <n v="9"/>
-    <n v="28.999999999999996"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0157"/>
-    <s v="Individual"/>
-    <s v="Erika"/>
-    <s v="Steward"/>
-    <n v="52"/>
-    <s v="46-55"/>
-    <n v="1955"/>
-    <n v="8"/>
-    <n v="7"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0118"/>
-    <s v="Individual"/>
-    <s v="Dangelo"/>
-    <s v="Shea"/>
-    <n v="53"/>
-    <s v="46-55"/>
-    <n v="1954"/>
-    <n v="2"/>
-    <n v="27"/>
-    <s v="M"/>
-    <x v="2"/>
-    <s v="Arizona"/>
-    <s v="Investment"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0119"/>
-    <s v="Individual"/>
-    <s v="Miguel"/>
-    <s v="Walter"/>
-    <n v="53"/>
-    <s v="46-55"/>
-    <n v="1954"/>
-    <n v="1"/>
-    <n v="7"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Arizona"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0033"/>
-    <s v="Individual"/>
-    <s v="Alanna"/>
-    <s v="Hess"/>
-    <n v="54"/>
-    <s v="46-55"/>
-    <n v="1952"/>
-    <n v="6"/>
-    <n v="19"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="Nevada"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0100"/>
-    <s v="Individual"/>
-    <s v="Simon"/>
-    <s v="Bennett"/>
-    <n v="54"/>
-    <s v="46-55"/>
-    <n v="1953"/>
-    <n v="6"/>
-    <n v="9"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Colorado"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0133"/>
-    <s v="Individual"/>
-    <s v="Ivan"/>
-    <s v="Bright"/>
-    <n v="54"/>
-    <s v="46-55"/>
-    <n v="1953"/>
-    <n v="9"/>
-    <n v="15"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0175"/>
-    <s v="Individual"/>
-    <s v="Madeline"/>
-    <s v="Michael"/>
-    <n v="54"/>
-    <s v="46-55"/>
-    <n v="1953"/>
-    <n v="7"/>
-    <n v="30"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0008"/>
-    <s v="Individual"/>
-    <s v="Arthur"/>
-    <s v="Bray"/>
-    <n v="55"/>
-    <s v="46-55"/>
-    <n v="1949"/>
-    <n v="7.0000000000000009"/>
-    <n v="14"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Utah"/>
-    <s v="Investment"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0023"/>
-    <s v="Individual"/>
-    <s v="Bennett"/>
-    <s v="Chen"/>
-    <n v="55"/>
-    <s v="46-55"/>
-    <n v="1950"/>
-    <n v="7.0000000000000009"/>
-    <n v="18"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Nevada"/>
-    <s v="Home"/>
-    <n v="2"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0108"/>
-    <s v="Individual"/>
-    <s v="Van"/>
-    <s v="Charles"/>
-    <n v="55"/>
-    <s v="46-55"/>
-    <n v="1952"/>
-    <n v="5"/>
-    <n v="15"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Colorado"/>
-    <s v="Home"/>
-    <n v="2"/>
-    <s v="Yes"/>
-    <s v="Client"/>
-  </r>
-  <r>
-    <s v="C0109"/>
-    <s v="Individual"/>
-    <s v="Rachel"/>
-    <s v="Cross"/>
-    <n v="55"/>
-    <s v="46-55"/>
-    <n v="1952"/>
-    <n v="6"/>
-    <n v="18"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0145"/>
-    <s v="Individual"/>
-    <s v="Augustus"/>
-    <s v="Hinton"/>
-    <n v="55"/>
-    <s v="46-55"/>
-    <n v="1953"/>
-    <n v="2"/>
-    <n v="3"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Nevada"/>
-    <s v="Investment"/>
-    <n v="2"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0145"/>
-    <s v="Individual"/>
-    <s v="Augustus"/>
-    <s v="Hinton"/>
-    <n v="55"/>
-    <s v="46-55"/>
-    <n v="1953"/>
-    <n v="2"/>
-    <n v="3"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Nevada"/>
-    <s v="Investment"/>
-    <n v="2"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0003"/>
-    <s v="Individual"/>
-    <s v="Avah"/>
-    <s v="Huang"/>
-    <n v="56"/>
-    <s v="56-65"/>
-    <n v="1948"/>
-    <n v="4"/>
-    <n v="23"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0004"/>
-    <s v="Individual"/>
-    <s v="Nora"/>
-    <s v="Lynch"/>
-    <n v="56"/>
-    <s v="56-65"/>
-    <n v="1948"/>
-    <n v="4"/>
-    <n v="23"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0024"/>
-    <s v="Individual"/>
-    <s v="Irvin"/>
-    <s v="Ellis"/>
-    <n v="56"/>
-    <s v="56-65"/>
-    <n v="1949"/>
-    <n v="11"/>
-    <n v="14"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0030"/>
-    <s v="Individual"/>
-    <s v="Aiyana"/>
-    <s v="Christensen"/>
-    <n v="56"/>
-    <s v="56-65"/>
-    <n v="1949"/>
-    <n v="1"/>
-    <n v="16"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0147"/>
-    <s v="Individual"/>
-    <s v="Parker"/>
-    <s v="Poole"/>
-    <n v="56"/>
-    <s v="56-65"/>
-    <n v="1951"/>
-    <n v="11"/>
-    <n v="10"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0002"/>
-    <s v="Individual"/>
-    <s v="Jack"/>
-    <s v="Anderson"/>
-    <n v="57"/>
-    <s v="56-65"/>
-    <n v="1947"/>
-    <n v="2"/>
-    <n v="13"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0031"/>
-    <s v="Individual"/>
-    <s v="Cedric"/>
-    <s v="Goodwin"/>
-    <n v="57"/>
-    <s v="56-65"/>
-    <n v="1948"/>
-    <n v="2"/>
-    <n v="20"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Utah"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Client"/>
-  </r>
-  <r>
-    <s v="C0059"/>
-    <s v="Individual"/>
-    <s v="Elena"/>
-    <s v="Petrova"/>
-    <n v="57"/>
-    <s v="56-65"/>
-    <n v="1949"/>
-    <n v="6"/>
-    <n v="22"/>
-    <s v="F"/>
-    <x v="3"/>
-    <m/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0140"/>
-    <s v="Individual"/>
-    <s v="Aniya"/>
-    <s v="Miller"/>
-    <n v="57"/>
-    <s v="56-65"/>
-    <n v="1950"/>
-    <n v="15"/>
-    <n v="2"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="Nevada"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0043"/>
-    <s v="Individual"/>
-    <s v="Kayley"/>
-    <s v="Nielsen"/>
-    <n v="59"/>
-    <s v="56-65"/>
-    <n v="1947"/>
-    <n v="4"/>
-    <n v="27"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="Arizona"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0078"/>
-    <s v="Individual"/>
-    <s v="Zaiden"/>
-    <s v="Merritt"/>
-    <n v="59"/>
-    <s v="56-65"/>
-    <n v="1948"/>
-    <n v="2"/>
-    <n v="23"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Wyoming"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0124"/>
-    <s v="Individual"/>
-    <s v="Sonia"/>
-    <s v="Choi"/>
-    <n v="59"/>
-    <s v="56-65"/>
-    <n v="1948"/>
-    <n v="11"/>
-    <n v="9"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="Oregon"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0049"/>
-    <s v="Individual"/>
-    <s v="Trey"/>
-    <s v="Strong"/>
-    <n v="48"/>
-    <s v="46-55"/>
-    <n v="1958"/>
-    <n v="12"/>
-    <n v="20"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0049"/>
-    <s v="Individual"/>
-    <s v="Trey"/>
-    <s v="Strong"/>
-    <n v="48"/>
-    <s v="46-55"/>
-    <n v="1958"/>
-    <n v="12"/>
-    <n v="20"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0079"/>
-    <s v="Individual"/>
-    <s v="Xavier"/>
-    <s v="Faulkner"/>
-    <n v="60"/>
-    <s v="56-65"/>
-    <n v="1947"/>
-    <n v="5"/>
-    <n v="24"/>
-    <s v="M"/>
-    <x v="7"/>
-    <m/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0079"/>
-    <s v="Individual"/>
-    <s v="Xavier"/>
-    <s v="Faulkner"/>
-    <n v="60"/>
-    <s v="56-65"/>
-    <n v="1947"/>
-    <n v="5"/>
-    <n v="24"/>
-    <s v="M"/>
-    <x v="7"/>
-    <m/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0079"/>
-    <s v="Individual"/>
-    <s v="Xavier"/>
-    <s v="Faulkner"/>
-    <n v="60"/>
-    <s v="56-65"/>
-    <n v="1947"/>
-    <n v="5"/>
-    <n v="24"/>
-    <s v="M"/>
-    <x v="7"/>
-    <m/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0079"/>
-    <s v="Individual"/>
-    <s v="Xavier"/>
-    <s v="Faulkner"/>
-    <n v="60"/>
-    <s v="56-65"/>
-    <n v="1947"/>
-    <n v="5"/>
-    <n v="24"/>
-    <s v="M"/>
-    <x v="7"/>
-    <m/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0079"/>
-    <s v="Individual"/>
-    <s v="Xavier"/>
-    <s v="Faulkner"/>
-    <n v="60"/>
-    <s v="56-65"/>
-    <n v="1947"/>
-    <n v="5"/>
-    <n v="24"/>
-    <s v="M"/>
-    <x v="7"/>
-    <m/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0079"/>
-    <s v="Individual"/>
-    <s v="Xavier"/>
-    <s v="Faulkner"/>
-    <n v="60"/>
-    <s v="56-65"/>
-    <n v="1947"/>
-    <n v="5"/>
-    <n v="24"/>
-    <s v="M"/>
-    <x v="7"/>
-    <m/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0079"/>
-    <s v="Individual"/>
-    <s v="Xavier"/>
-    <s v="Faulkner"/>
-    <n v="60"/>
-    <s v="56-65"/>
-    <n v="1947"/>
-    <n v="5"/>
-    <n v="24"/>
-    <s v="M"/>
-    <x v="7"/>
-    <m/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0013"/>
-    <s v="Individual"/>
-    <s v="Franklin"/>
-    <s v="Mack"/>
-    <n v="61"/>
-    <s v="56-65"/>
-    <n v="1943"/>
-    <n v="6"/>
-    <n v="18"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Virginia"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0139"/>
-    <s v="Individual"/>
-    <s v="Logan"/>
-    <s v="Simmons"/>
-    <n v="61"/>
-    <s v="56-65"/>
-    <n v="1946"/>
-    <n v="9"/>
-    <n v="14"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0154"/>
-    <s v="Individual"/>
-    <s v="Sidney"/>
-    <s v="Cline"/>
-    <n v="64"/>
-    <s v="56-65"/>
-    <n v="1943"/>
-    <n v="7"/>
-    <n v="24"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0045"/>
-    <s v="Individual"/>
-    <s v="Matilda"/>
-    <s v="Madden"/>
-    <n v="65"/>
-    <s v="56-65"/>
-    <n v="1941"/>
-    <n v="3"/>
-    <n v="2.9999999999999996"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="Colorado"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0134"/>
-    <s v="Individual"/>
-    <s v="Yesenia"/>
-    <s v="Marquez"/>
-    <n v="65"/>
-    <s v="56-65"/>
-    <n v="1942"/>
-    <n v="7.0000000000000009"/>
-    <n v="23"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="Arizona"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0138"/>
-    <s v="Individual"/>
-    <s v="Colin"/>
-    <s v="Campos"/>
-    <n v="65"/>
-    <s v="56-65"/>
-    <n v="1942"/>
-    <n v="4"/>
-    <n v="14"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0158"/>
-    <s v="Individual"/>
-    <s v="Erika"/>
-    <s v="Gallagher"/>
-    <n v="65"/>
-    <s v="56-65"/>
-    <n v="1942"/>
-    <n v="7.0000000000000009"/>
-    <n v="19"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="1"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0036"/>
-    <s v="Individual"/>
-    <s v="Jair"/>
-    <s v="Johns"/>
-    <n v="66"/>
-    <s v="65+"/>
-    <n v="1940"/>
-    <n v="3"/>
-    <n v="5"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0074"/>
-    <s v="Individual"/>
-    <s v="Jaylynn"/>
-    <s v="Hickman"/>
-    <n v="66"/>
-    <s v="65+"/>
-    <n v="1941"/>
-    <n v="8"/>
-    <n v="19"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Client"/>
-  </r>
-  <r>
-    <s v="C0120"/>
-    <s v="Individual"/>
-    <s v="Jack"/>
-    <s v="Hanson"/>
-    <n v="66"/>
-    <s v="65+"/>
-    <n v="1941"/>
-    <n v="12"/>
-    <n v="1"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0120"/>
-    <s v="Individual"/>
-    <s v="Jack"/>
-    <s v="Hanson"/>
-    <n v="66"/>
-    <s v="65+"/>
-    <n v="1941"/>
-    <n v="12"/>
-    <n v="1"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0005"/>
-    <s v="Individual"/>
-    <s v="Rodolfo"/>
-    <s v="Gibson"/>
-    <n v="67"/>
-    <s v="65+"/>
-    <n v="1937"/>
-    <n v="1"/>
-    <n v="20"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Nevada"/>
-    <s v="Home"/>
-    <n v="2"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0032"/>
-    <s v="Individual"/>
-    <s v="Olivia"/>
-    <s v="Oconnell"/>
-    <n v="67"/>
-    <s v="65+"/>
-    <n v="1939"/>
-    <n v="9"/>
-    <n v="2.9999999999999996"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0126"/>
-    <s v="Individual"/>
-    <s v="Crystal"/>
-    <s v="Wyatt"/>
-    <n v="67"/>
-    <s v="65+"/>
-    <n v="1939"/>
-    <n v="6"/>
-    <n v="30"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="Oregon"/>
-    <s v="Investment"/>
-    <n v="3"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0106"/>
-    <s v="Individual"/>
-    <s v="Ruben"/>
-    <s v="Melton"/>
-    <n v="68"/>
-    <s v="65+"/>
-    <n v="1939"/>
-    <n v="3"/>
-    <n v="5"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Utah"/>
-    <s v="Investment"/>
-    <n v="2"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0115"/>
-    <s v="Individual"/>
-    <s v="Issac"/>
-    <s v="Edwards"/>
-    <n v="69"/>
-    <s v="65+"/>
-    <n v="1938"/>
-    <n v="10"/>
-    <n v="28.999999999999996"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0115"/>
-    <s v="Individual"/>
-    <s v="Issac"/>
-    <s v="Edwards"/>
-    <n v="69"/>
-    <s v="65+"/>
-    <n v="1938"/>
-    <n v="10"/>
-    <n v="28.999999999999996"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0129"/>
-    <s v="Individual"/>
-    <s v="Jesus"/>
-    <s v="Obrien"/>
-    <n v="69"/>
-    <s v="65+"/>
-    <n v="1938"/>
-    <n v="6"/>
-    <n v="9"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Oregon"/>
-    <s v="Investment"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0129"/>
-    <s v="Individual"/>
-    <s v="Jesus"/>
-    <s v="Obrien"/>
-    <n v="69"/>
-    <s v="65+"/>
-    <n v="1938"/>
-    <n v="6"/>
-    <n v="9"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Oregon"/>
-    <s v="Investment"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0103"/>
-    <s v="Individual"/>
-    <s v="Jamal"/>
-    <s v="Mueller"/>
-    <n v="71"/>
-    <s v="65+"/>
-    <n v="1936"/>
-    <n v="8"/>
-    <n v="13"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Oregon"/>
-    <s v="Investment"/>
-    <n v="2"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0103"/>
-    <s v="Individual"/>
-    <s v="Jamal"/>
-    <s v="Mueller"/>
-    <n v="71"/>
-    <s v="65+"/>
-    <n v="1936"/>
-    <n v="8"/>
-    <n v="13"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="Oregon"/>
-    <s v="Investment"/>
-    <n v="2"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0021"/>
-    <s v="Individual"/>
-    <s v="Kaylin"/>
-    <s v="Villarreal"/>
-    <n v="73"/>
-    <s v="65+"/>
-    <n v="1932"/>
-    <n v="6"/>
-    <n v="13"/>
-    <s v="F"/>
-    <x v="3"/>
-    <m/>
-    <s v="Investment"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0148"/>
-    <s v="Individual"/>
-    <s v="Myah"/>
-    <s v="Roman"/>
-    <n v="73"/>
-    <s v="65+"/>
-    <n v="1933"/>
-    <n v="5"/>
-    <n v="5"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0172"/>
-    <s v="Individual"/>
-    <s v="Henry"/>
-    <s v="Kennedy"/>
-    <n v="73"/>
-    <s v="65+"/>
-    <n v="1933"/>
-    <n v="6"/>
-    <n v="8"/>
-    <s v="M"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="4"/>
-    <s v="Yes"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0104"/>
-    <s v="Individual"/>
-    <s v="Diana"/>
-    <s v="Hunt"/>
-    <n v="76"/>
-    <s v="65+"/>
-    <n v="1931"/>
-    <n v="2"/>
-    <n v="13"/>
-    <s v="F"/>
-    <x v="0"/>
-    <s v="Arizona"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <s v=" "/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="8"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <s v="C0001"/>
-    <s v="Firm"/>
-    <s v="Kamd"/>
-    <s v="Co"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <m/>
-    <m/>
-    <s v="N/A"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Agency"/>
-  </r>
-  <r>
-    <s v="C0012"/>
-    <s v="Firm"/>
-    <s v="Bridger CAL"/>
-    <s v="Co"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <m/>
-    <m/>
-    <s v="N/A"/>
-    <x v="0"/>
-    <s v="Nevada"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0012"/>
-    <s v="Firm"/>
-    <s v="Bridger CAL"/>
-    <s v="Co"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <m/>
-    <m/>
-    <s v="N/A"/>
-    <x v="0"/>
-    <s v="Nevada"/>
-    <s v="Investment"/>
-    <n v="4"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0025"/>
-    <s v="Firm"/>
-    <s v="Abdiel"/>
-    <s v="Co"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <m/>
-    <m/>
-    <s v="N/A"/>
-    <x v="0"/>
-    <s v="Nevada"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0029"/>
-    <s v="Firm"/>
-    <s v="Kenyon"/>
-    <s v="Co"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <m/>
-    <m/>
-    <s v="N/A"/>
-    <x v="0"/>
-    <s v="Nevada"/>
-    <s v="Investment"/>
-    <n v="1"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0029"/>
-    <s v="Firm"/>
-    <s v="Kenyon"/>
-    <s v="Co"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <m/>
-    <m/>
-    <s v="N/A"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="1"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0055"/>
-    <s v="Firm"/>
-    <s v="Kylax"/>
-    <s v="Co"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <m/>
-    <m/>
-    <s v="N/A"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0121"/>
-    <s v="Firm"/>
-    <s v="Esther"/>
-    <s v="Co"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <m/>
-    <m/>
-    <s v="N/A"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Home"/>
-    <n v="3"/>
-    <s v="Yes"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0174"/>
-    <s v="Firm"/>
-    <s v="Marleez"/>
-    <s v="Co"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <m/>
-    <m/>
-    <s v="N/A"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0174"/>
-    <s v="Firm"/>
-    <s v="Marleez"/>
-    <s v="Co"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <m/>
-    <m/>
-    <s v="N/A"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0174"/>
-    <s v="Firm"/>
-    <s v="Marleez"/>
-    <s v="Co"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <m/>
-    <m/>
-    <s v="N/A"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0174"/>
-    <s v="Firm"/>
-    <s v="Marleez"/>
-    <s v="Co"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <m/>
-    <m/>
-    <s v="N/A"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0174"/>
-    <s v="Firm"/>
-    <s v="Marleez"/>
-    <s v="Co"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <m/>
-    <m/>
-    <s v="N/A"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0174"/>
-    <s v="Firm"/>
-    <s v="Marleez"/>
-    <s v="Co"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <m/>
-    <m/>
-    <s v="N/A"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0174"/>
-    <s v="Firm"/>
-    <s v="Marleez"/>
-    <s v="Co"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <m/>
-    <m/>
-    <s v="N/A"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0174"/>
-    <s v="Firm"/>
-    <s v="Marleez"/>
-    <s v="Co"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <m/>
-    <m/>
-    <s v="N/A"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-  <r>
-    <s v="C0174"/>
-    <s v="Firm"/>
-    <s v="Marleez"/>
-    <s v="Co"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <s v="N/A"/>
-    <m/>
-    <m/>
-    <s v="N/A"/>
-    <x v="0"/>
-    <s v="California"/>
-    <s v="Investment"/>
-    <n v="5"/>
-    <s v="No"/>
-    <s v="Website"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DF112065-EABF-45BF-A1FE-F19B866AD767}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="10">
-        <item x="2"/>
-        <item x="7"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="8"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="10"/>
-  </rowFields>
-  <rowItems count="10">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Customer ID" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -11078,35 +7377,35 @@
       <c r="W3" s="14"/>
     </row>
     <row r="4" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="66" t="s">
         <v>528</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="L4" s="67" t="s">
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="L4" s="66" t="s">
         <v>529</v>
       </c>
-      <c r="M4" s="67"/>
-      <c r="N4" s="67"/>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="67"/>
-      <c r="V4" s="67"/>
-      <c r="W4" s="67"/>
-      <c r="X4" s="67"/>
-      <c r="Y4" s="67"/>
-      <c r="Z4" s="67"/>
-      <c r="AA4" s="67"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="66"/>
+      <c r="R4" s="66"/>
+      <c r="S4" s="66"/>
+      <c r="T4" s="66"/>
+      <c r="U4" s="66"/>
+      <c r="V4" s="66"/>
+      <c r="W4" s="66"/>
+      <c r="X4" s="66"/>
+      <c r="Y4" s="66"/>
+      <c r="Z4" s="66"/>
+      <c r="AA4" s="66"/>
     </row>
     <row r="5" spans="2:27" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="35" t="s">
@@ -48978,168 +45277,168 @@
       <c r="B7" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="65" t="s">
-        <v>577</v>
-      </c>
-      <c r="D7" s="65" t="s">
-        <v>578</v>
-      </c>
-      <c r="E7" s="65" t="s">
-        <v>579</v>
+      <c r="C7" s="64" t="s">
+        <v>573</v>
+      </c>
+      <c r="D7" s="64" t="s">
+        <v>574</v>
+      </c>
+      <c r="E7" s="64" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="63">
+      <c r="C8" s="62">
         <v>177</v>
       </c>
-      <c r="D8" s="64">
+      <c r="D8" s="63">
         <f t="shared" ref="D8:D15" si="0">C8/$C$16</f>
         <v>0.90769230769230769</v>
       </c>
-      <c r="E8" s="66">
+      <c r="E8" s="65">
         <f>D8</f>
         <v>0.90769230769230769</v>
       </c>
       <c r="J8" s="31"/>
     </row>
     <row r="9" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="63">
+      <c r="C9" s="62">
         <v>7</v>
       </c>
-      <c r="D9" s="64">
+      <c r="D9" s="63">
         <f t="shared" si="0"/>
         <v>3.5897435897435895E-2</v>
       </c>
-      <c r="E9" s="66">
+      <c r="E9" s="65">
         <f>E8+D9</f>
         <v>0.94358974358974357</v>
       </c>
       <c r="J9" s="31"/>
     </row>
     <row r="10" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="63">
+      <c r="C10" s="62">
         <v>4</v>
       </c>
-      <c r="D10" s="64">
+      <c r="D10" s="63">
         <f t="shared" si="0"/>
         <v>2.0512820512820513E-2</v>
       </c>
-      <c r="E10" s="66">
+      <c r="E10" s="65">
         <f t="shared" ref="E10:E15" si="1">E9+D10</f>
         <v>0.96410256410256412</v>
       </c>
       <c r="J10" s="31"/>
     </row>
     <row r="11" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="63">
+      <c r="C11" s="62">
         <v>2</v>
       </c>
-      <c r="D11" s="64">
+      <c r="D11" s="63">
         <f t="shared" si="0"/>
         <v>1.0256410256410256E-2</v>
       </c>
-      <c r="E11" s="66">
+      <c r="E11" s="65">
         <f t="shared" si="1"/>
         <v>0.97435897435897434</v>
       </c>
       <c r="J11" s="31"/>
     </row>
     <row r="12" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" s="62" t="s">
+      <c r="B12" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="63">
+      <c r="C12" s="62">
         <v>2</v>
       </c>
-      <c r="D12" s="64">
+      <c r="D12" s="63">
         <f t="shared" si="0"/>
         <v>1.0256410256410256E-2</v>
       </c>
-      <c r="E12" s="66">
+      <c r="E12" s="65">
         <f t="shared" si="1"/>
         <v>0.98461538461538456</v>
       </c>
       <c r="J12" s="31"/>
     </row>
     <row r="13" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="62" t="s">
+      <c r="B13" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="63">
+      <c r="C13" s="62">
         <v>1</v>
       </c>
-      <c r="D13" s="64">
+      <c r="D13" s="63">
         <f t="shared" si="0"/>
         <v>5.1282051282051282E-3</v>
       </c>
-      <c r="E13" s="66">
+      <c r="E13" s="65">
         <f t="shared" si="1"/>
         <v>0.98974358974358967</v>
       </c>
       <c r="J13" s="31"/>
     </row>
     <row r="14" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="62" t="s">
+      <c r="B14" s="61" t="s">
         <v>490</v>
       </c>
-      <c r="C14" s="63">
+      <c r="C14" s="62">
         <v>1</v>
       </c>
-      <c r="D14" s="64">
+      <c r="D14" s="63">
         <f t="shared" si="0"/>
         <v>5.1282051282051282E-3</v>
       </c>
-      <c r="E14" s="66">
+      <c r="E14" s="65">
         <f t="shared" si="1"/>
         <v>0.99487179487179478</v>
       </c>
       <c r="J14" s="31"/>
     </row>
     <row r="15" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B15" s="62" t="s">
+      <c r="B15" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="63">
+      <c r="C15" s="62">
         <v>1</v>
       </c>
-      <c r="D15" s="64">
+      <c r="D15" s="63">
         <f t="shared" si="0"/>
         <v>5.1282051282051282E-3</v>
       </c>
-      <c r="E15" s="66">
+      <c r="E15" s="65">
         <f t="shared" si="1"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="J15" s="31"/>
     </row>
     <row r="16" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B16" s="62" t="s">
-        <v>576</v>
-      </c>
-      <c r="C16" s="63">
+      <c r="B16" s="61" t="s">
+        <v>572</v>
+      </c>
+      <c r="C16" s="62">
         <f>SUM(C8:C15)</f>
         <v>195</v>
       </c>
-      <c r="D16" s="64">
+      <c r="D16" s="63">
         <f>SUM(D8:D15)</f>
         <v>0.99999999999999989</v>
       </c>
       <c r="J16" s="31"/>
     </row>
     <row r="17" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="62"/>
+      <c r="B17" s="61"/>
       <c r="J17" s="31"/>
     </row>
     <row r="18" spans="2:10" ht="15" x14ac:dyDescent="0.25">
@@ -49615,7 +45914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:X189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -49722,7 +46021,7 @@
     </row>
     <row r="8" spans="2:24" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="32" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="C8" s="52">
         <f>AVERAGE('365RE'!$I$6:$I$272)</f>
@@ -49732,7 +46031,7 @@
     </row>
     <row r="9" spans="2:24" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="32" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="C9" s="52">
         <f>MEDIAN('365RE'!$I$6:$I$272)</f>
@@ -49742,7 +46041,7 @@
     </row>
     <row r="10" spans="2:24" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="32" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="C10" s="52">
         <f>_xlfn.MODE.SNGL('365RE'!$I$6:$I$272)</f>
@@ -49752,7 +46051,7 @@
     </row>
     <row r="11" spans="2:24" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="32" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="C11" s="52">
         <f>SKEW('365RE'!$I$6:$I$272)</f>
@@ -49762,7 +46061,7 @@
     </row>
     <row r="12" spans="2:24" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="32" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="C12" s="52">
         <f>_xlfn.VAR.S('365RE'!$I$6:$I$272)</f>
@@ -49772,7 +46071,7 @@
     </row>
     <row r="13" spans="2:24" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="32" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="C13" s="52">
         <f>_xlfn.STDEV.S('365RE'!$I$6:$I$272)</f>
@@ -49788,7 +46087,7 @@
     </row>
     <row r="16" spans="2:24" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="59" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="H16" s="31"/>
     </row>
@@ -50323,15 +46622,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2" style="32" customWidth="1"/>
     <col min="2" max="2" width="19" style="32" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="32" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="8.85546875" style="32"/>
   </cols>
   <sheetData>
@@ -50359,118 +46658,36 @@
       <c r="B6" s="42"/>
       <c r="C6" s="44"/>
     </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="32" t="s">
+        <v>583</v>
+      </c>
+      <c r="C7" s="32">
+        <f>_xlfn.COVARIANCE.S('365RE'!$H$6:$H$272,'365RE'!$I$6:$I$272)</f>
+        <v>24147721.725818869</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="32" t="s">
+        <v>584</v>
+      </c>
+      <c r="C8" s="32">
+        <f>CORREL('365RE'!$H$6:$H$272,'365RE'!$I$6:$I$272)</f>
+        <v>0.95108737743161964</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="32" t="s">
+        <v>585</v>
+      </c>
+    </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B25" s="26"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="B1:B2" xr:uid="{00000000-0002-0000-0400-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D9A324-451E-4348-9433-8E2B0CEB1881}">
-  <dimension ref="A3:B13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
-        <v>572</v>
-      </c>
-      <c r="B3" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="62" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="63">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="62" t="s">
-        <v>490</v>
-      </c>
-      <c r="B5" s="63">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="62" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="62" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="62" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="63">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="63">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="62" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="63">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="62" t="s">
-        <v>573</v>
-      </c>
-      <c r="B12" s="63"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="62" t="s">
-        <v>574</v>
-      </c>
-      <c r="B13" s="63">
-        <v>195</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>